<commit_message>
git snapshot 24.10.2024 06:01
</commit_message>
<xml_diff>
--- a/docs/ru/cases/performance-testing/assets/disk_testing.xlsx
+++ b/docs/ru/cases/performance-testing/assets/disk_testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11850"/>
+    <workbookView windowWidth="21000" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Parameters</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>BS=4k, iodepth=32</t>
-    </r>
+    <t>BS=4k, iodepth=32</t>
   </si>
   <si>
     <t>BS=64k, iodepth=32</t>
@@ -50,15 +41,7 @@
     <t>Random Read</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>clat percentiles (usec): 99.00th</t>
-    </r>
+    <t>clat percentiles (usec): 99.00th</t>
   </si>
   <si>
     <t>bw (KiB/s): avg</t>
@@ -71,9 +54,6 @@
   </si>
   <si>
     <t>SQ Read</t>
-  </si>
-  <si>
-    <t>clat percentiles (usec): 99.00th</t>
   </si>
   <si>
     <t>-</t>
@@ -113,7 +93,7 @@
     <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -124,20 +104,11 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF172B4D"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
@@ -150,9 +121,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Inherit"/>
+      <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,25 +142,6 @@
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="-apple-system"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1059,19 +1022,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1080,131 +1052,122 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1215,89 +1178,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1306,37 +1266,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1345,37 +1308,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1856,7 +1822,7 @@
   <dimension ref="A1:F1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
@@ -1923,7 +1889,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" customHeight="1" spans="1:6">
@@ -1932,8 +1898,8 @@
         <v>5</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" customHeight="1" spans="1:6">
@@ -1942,32 +1908,32 @@
         <v>6</v>
       </c>
       <c r="C7" s="19"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" customHeight="1" spans="1:6">
@@ -1976,42 +1942,42 @@
         <v>5</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="17"/>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="11"/>
     </row>
     <row r="14" customHeight="1" spans="1:6">
@@ -2020,38 +1986,38 @@
         <v>5</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="11"/>
     </row>
     <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="17"/>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="27"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="11"/>
     </row>
     <row r="16" customHeight="1" spans="1:6">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42" t="s">
+      <c r="C16" s="39" t="s">
         <v>10</v>
       </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" customHeight="1" spans="1:6">
-      <c r="A17" s="30"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="43"/>
       <c r="C17" s="44" t="s">
         <v>5</v>
@@ -2061,7 +2027,7 @@
       <c r="F17" s="11"/>
     </row>
     <row r="18" customHeight="1" spans="1:6">
-      <c r="A18" s="30"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="47"/>
       <c r="C18" s="48" t="s">
         <v>6</v>
@@ -2071,21 +2037,21 @@
       <c r="F18" s="11"/>
     </row>
     <row r="19" customHeight="1" spans="1:6">
-      <c r="A19" s="30"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="11"/>
     </row>
     <row r="20" customHeight="1" spans="1:6">
-      <c r="A20" s="30"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="43"/>
       <c r="C20" s="44" t="s">
         <v>5</v>
@@ -2095,33 +2061,33 @@
       <c r="F20" s="11"/>
     </row>
     <row r="21" customHeight="1" spans="1:6">
-      <c r="A21" s="34"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" customHeight="1" spans="1:6">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42" t="s">
+      <c r="C22" s="39" t="s">
         <v>10</v>
       </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="F22" s="11"/>
     </row>
     <row r="23" customHeight="1" spans="1:6">
-      <c r="A23" s="30"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="43"/>
       <c r="C23" s="44" t="s">
         <v>5</v>
@@ -2131,7 +2097,7 @@
       <c r="F23" s="11"/>
     </row>
     <row r="24" customHeight="1" spans="1:6">
-      <c r="A24" s="30"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="47"/>
       <c r="C24" s="48" t="s">
         <v>6</v>
@@ -2141,21 +2107,21 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" customHeight="1" spans="1:6">
-      <c r="A25" s="30"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="11"/>
     </row>
     <row r="26" customHeight="1" spans="1:6">
-      <c r="A26" s="30"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="43"/>
       <c r="C26" s="44" t="s">
         <v>5</v>
@@ -2165,61 +2131,61 @@
       <c r="F26" s="11"/>
     </row>
     <row r="27" customHeight="1" spans="1:6">
-      <c r="A27" s="34"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="55"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" customHeight="1" spans="1:6">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" customHeight="1" spans="1:6">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" customHeight="1" spans="1:6">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
       <c r="F30" s="11"/>
     </row>
     <row r="31" customHeight="1" spans="1:6">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" customHeight="1" spans="1:6">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" customHeight="1" spans="1:6">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" customHeight="1" spans="1:6">
@@ -2234,2986 +2200,2986 @@
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" customHeight="1" spans="1:6">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" customHeight="1" spans="1:6">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" customHeight="1" spans="1:4">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="57"/>
+      <c r="D38" s="58"/>
     </row>
     <row r="39" customHeight="1" spans="1:1">
-      <c r="A39" s="58"/>
+      <c r="A39" s="59"/>
     </row>
     <row r="40" customHeight="1" spans="1:1">
-      <c r="A40" s="58"/>
+      <c r="A40" s="59"/>
     </row>
     <row r="41" customHeight="1" spans="1:1">
-      <c r="A41" s="58"/>
+      <c r="A41" s="59"/>
     </row>
     <row r="42" customHeight="1" spans="1:1">
-      <c r="A42" s="58"/>
+      <c r="A42" s="59"/>
     </row>
     <row r="43" customHeight="1" spans="1:1">
-      <c r="A43" s="58"/>
+      <c r="A43" s="59"/>
     </row>
     <row r="44" customHeight="1" spans="1:1">
-      <c r="A44" s="58"/>
+      <c r="A44" s="59"/>
     </row>
     <row r="45" customHeight="1" spans="1:1">
-      <c r="A45" s="58"/>
+      <c r="A45" s="59"/>
     </row>
     <row r="46" customHeight="1" spans="1:1">
-      <c r="A46" s="58"/>
+      <c r="A46" s="59"/>
     </row>
     <row r="47" customHeight="1" spans="1:1">
-      <c r="A47" s="58"/>
+      <c r="A47" s="59"/>
     </row>
     <row r="48" customHeight="1" spans="1:1">
-      <c r="A48" s="58"/>
+      <c r="A48" s="59"/>
     </row>
     <row r="49" customHeight="1" spans="1:1">
-      <c r="A49" s="58"/>
+      <c r="A49" s="59"/>
     </row>
     <row r="50" customHeight="1" spans="1:1">
-      <c r="A50" s="58"/>
+      <c r="A50" s="59"/>
     </row>
     <row r="51" customHeight="1" spans="1:1">
-      <c r="A51" s="58"/>
+      <c r="A51" s="59"/>
     </row>
     <row r="52" customHeight="1" spans="1:1">
-      <c r="A52" s="58"/>
+      <c r="A52" s="59"/>
     </row>
     <row r="53" customHeight="1" spans="1:1">
-      <c r="A53" s="58"/>
+      <c r="A53" s="59"/>
     </row>
     <row r="54" customHeight="1" spans="1:1">
-      <c r="A54" s="58"/>
+      <c r="A54" s="59"/>
     </row>
     <row r="55" customHeight="1" spans="1:1">
-      <c r="A55" s="58"/>
+      <c r="A55" s="59"/>
     </row>
     <row r="56" customHeight="1" spans="1:1">
-      <c r="A56" s="58"/>
+      <c r="A56" s="59"/>
     </row>
     <row r="57" customHeight="1" spans="1:1">
-      <c r="A57" s="58"/>
+      <c r="A57" s="59"/>
     </row>
     <row r="58" customHeight="1" spans="1:1">
-      <c r="A58" s="58"/>
+      <c r="A58" s="59"/>
     </row>
     <row r="59" customHeight="1" spans="1:1">
-      <c r="A59" s="58"/>
+      <c r="A59" s="59"/>
     </row>
     <row r="60" customHeight="1" spans="1:1">
-      <c r="A60" s="58"/>
+      <c r="A60" s="59"/>
     </row>
     <row r="61" customHeight="1" spans="1:1">
-      <c r="A61" s="58"/>
+      <c r="A61" s="59"/>
     </row>
     <row r="62" customHeight="1" spans="1:1">
-      <c r="A62" s="58"/>
+      <c r="A62" s="59"/>
     </row>
     <row r="63" customHeight="1" spans="1:1">
-      <c r="A63" s="58"/>
+      <c r="A63" s="59"/>
     </row>
     <row r="64" customHeight="1" spans="1:1">
-      <c r="A64" s="58"/>
+      <c r="A64" s="59"/>
     </row>
     <row r="65" customHeight="1" spans="1:1">
-      <c r="A65" s="58"/>
+      <c r="A65" s="59"/>
     </row>
     <row r="66" customHeight="1" spans="1:1">
-      <c r="A66" s="58"/>
+      <c r="A66" s="59"/>
     </row>
     <row r="67" customHeight="1" spans="1:1">
-      <c r="A67" s="58"/>
+      <c r="A67" s="59"/>
     </row>
     <row r="68" customHeight="1" spans="1:1">
-      <c r="A68" s="58"/>
+      <c r="A68" s="59"/>
     </row>
     <row r="69" customHeight="1" spans="1:1">
-      <c r="A69" s="58"/>
+      <c r="A69" s="59"/>
     </row>
     <row r="70" customHeight="1" spans="1:1">
-      <c r="A70" s="58"/>
+      <c r="A70" s="59"/>
     </row>
     <row r="71" customHeight="1" spans="1:1">
-      <c r="A71" s="58"/>
+      <c r="A71" s="59"/>
     </row>
     <row r="72" customHeight="1" spans="1:1">
-      <c r="A72" s="58"/>
+      <c r="A72" s="59"/>
     </row>
     <row r="73" customHeight="1" spans="1:1">
-      <c r="A73" s="58"/>
+      <c r="A73" s="59"/>
     </row>
     <row r="74" customHeight="1" spans="1:1">
-      <c r="A74" s="58"/>
+      <c r="A74" s="59"/>
     </row>
     <row r="75" customHeight="1" spans="1:1">
-      <c r="A75" s="58"/>
+      <c r="A75" s="59"/>
     </row>
     <row r="76" customHeight="1" spans="1:1">
-      <c r="A76" s="58"/>
+      <c r="A76" s="59"/>
     </row>
     <row r="77" customHeight="1" spans="1:1">
-      <c r="A77" s="58"/>
+      <c r="A77" s="59"/>
     </row>
     <row r="78" customHeight="1" spans="1:1">
-      <c r="A78" s="58"/>
+      <c r="A78" s="59"/>
     </row>
     <row r="79" customHeight="1" spans="1:1">
-      <c r="A79" s="58"/>
+      <c r="A79" s="59"/>
     </row>
     <row r="80" customHeight="1" spans="1:1">
-      <c r="A80" s="58"/>
+      <c r="A80" s="59"/>
     </row>
     <row r="81" customHeight="1" spans="1:1">
-      <c r="A81" s="58"/>
+      <c r="A81" s="59"/>
     </row>
     <row r="82" customHeight="1" spans="1:1">
-      <c r="A82" s="58"/>
+      <c r="A82" s="59"/>
     </row>
     <row r="83" customHeight="1" spans="1:1">
-      <c r="A83" s="58"/>
+      <c r="A83" s="59"/>
     </row>
     <row r="84" customHeight="1" spans="1:1">
-      <c r="A84" s="58"/>
+      <c r="A84" s="59"/>
     </row>
     <row r="85" customHeight="1" spans="1:1">
-      <c r="A85" s="58"/>
+      <c r="A85" s="59"/>
     </row>
     <row r="86" customHeight="1" spans="1:1">
-      <c r="A86" s="58"/>
+      <c r="A86" s="59"/>
     </row>
     <row r="87" customHeight="1" spans="1:1">
-      <c r="A87" s="58"/>
+      <c r="A87" s="59"/>
     </row>
     <row r="88" customHeight="1" spans="1:1">
-      <c r="A88" s="58"/>
+      <c r="A88" s="59"/>
     </row>
     <row r="89" customHeight="1" spans="1:1">
-      <c r="A89" s="58"/>
+      <c r="A89" s="59"/>
     </row>
     <row r="90" customHeight="1" spans="1:1">
-      <c r="A90" s="58"/>
+      <c r="A90" s="59"/>
     </row>
     <row r="91" customHeight="1" spans="1:1">
-      <c r="A91" s="58"/>
+      <c r="A91" s="59"/>
     </row>
     <row r="92" customHeight="1" spans="1:1">
-      <c r="A92" s="58"/>
+      <c r="A92" s="59"/>
     </row>
     <row r="93" customHeight="1" spans="1:1">
-      <c r="A93" s="58"/>
+      <c r="A93" s="59"/>
     </row>
     <row r="94" customHeight="1" spans="1:1">
-      <c r="A94" s="58"/>
+      <c r="A94" s="59"/>
     </row>
     <row r="95" customHeight="1" spans="1:1">
-      <c r="A95" s="58"/>
+      <c r="A95" s="59"/>
     </row>
     <row r="96" customHeight="1" spans="1:1">
-      <c r="A96" s="58"/>
+      <c r="A96" s="59"/>
     </row>
     <row r="97" customHeight="1" spans="1:1">
-      <c r="A97" s="58"/>
+      <c r="A97" s="59"/>
     </row>
     <row r="98" customHeight="1" spans="1:1">
-      <c r="A98" s="58"/>
+      <c r="A98" s="59"/>
     </row>
     <row r="99" customHeight="1" spans="1:1">
-      <c r="A99" s="58"/>
+      <c r="A99" s="59"/>
     </row>
     <row r="100" customHeight="1" spans="1:1">
-      <c r="A100" s="58"/>
+      <c r="A100" s="59"/>
     </row>
     <row r="101" customHeight="1" spans="1:1">
-      <c r="A101" s="58"/>
+      <c r="A101" s="59"/>
     </row>
     <row r="102" customHeight="1" spans="1:1">
-      <c r="A102" s="58"/>
+      <c r="A102" s="59"/>
     </row>
     <row r="103" customHeight="1" spans="1:1">
-      <c r="A103" s="58"/>
+      <c r="A103" s="59"/>
     </row>
     <row r="104" customHeight="1" spans="1:1">
-      <c r="A104" s="58"/>
+      <c r="A104" s="59"/>
     </row>
     <row r="105" customHeight="1" spans="1:1">
-      <c r="A105" s="58"/>
+      <c r="A105" s="59"/>
     </row>
     <row r="106" customHeight="1" spans="1:1">
-      <c r="A106" s="58"/>
+      <c r="A106" s="59"/>
     </row>
     <row r="107" customHeight="1" spans="1:1">
-      <c r="A107" s="58"/>
+      <c r="A107" s="59"/>
     </row>
     <row r="108" customHeight="1" spans="1:1">
-      <c r="A108" s="58"/>
+      <c r="A108" s="59"/>
     </row>
     <row r="109" customHeight="1" spans="1:1">
-      <c r="A109" s="58"/>
+      <c r="A109" s="59"/>
     </row>
     <row r="110" customHeight="1" spans="1:1">
-      <c r="A110" s="58"/>
+      <c r="A110" s="59"/>
     </row>
     <row r="111" customHeight="1" spans="1:1">
-      <c r="A111" s="58"/>
+      <c r="A111" s="59"/>
     </row>
     <row r="112" customHeight="1" spans="1:1">
-      <c r="A112" s="58"/>
+      <c r="A112" s="59"/>
     </row>
     <row r="113" customHeight="1" spans="1:1">
-      <c r="A113" s="58"/>
+      <c r="A113" s="59"/>
     </row>
     <row r="114" customHeight="1" spans="1:1">
-      <c r="A114" s="58"/>
+      <c r="A114" s="59"/>
     </row>
     <row r="115" customHeight="1" spans="1:1">
-      <c r="A115" s="58"/>
+      <c r="A115" s="59"/>
     </row>
     <row r="116" customHeight="1" spans="1:1">
-      <c r="A116" s="58"/>
+      <c r="A116" s="59"/>
     </row>
     <row r="117" customHeight="1" spans="1:1">
-      <c r="A117" s="58"/>
+      <c r="A117" s="59"/>
     </row>
     <row r="118" customHeight="1" spans="1:1">
-      <c r="A118" s="58"/>
+      <c r="A118" s="59"/>
     </row>
     <row r="119" customHeight="1" spans="1:1">
-      <c r="A119" s="58"/>
+      <c r="A119" s="59"/>
     </row>
     <row r="120" customHeight="1" spans="1:1">
-      <c r="A120" s="58"/>
+      <c r="A120" s="59"/>
     </row>
     <row r="121" customHeight="1" spans="1:1">
-      <c r="A121" s="58"/>
+      <c r="A121" s="59"/>
     </row>
     <row r="122" customHeight="1" spans="1:1">
-      <c r="A122" s="58"/>
+      <c r="A122" s="59"/>
     </row>
     <row r="123" customHeight="1" spans="1:1">
-      <c r="A123" s="58"/>
+      <c r="A123" s="59"/>
     </row>
     <row r="124" customHeight="1" spans="1:1">
-      <c r="A124" s="58"/>
+      <c r="A124" s="59"/>
     </row>
     <row r="125" customHeight="1" spans="1:1">
-      <c r="A125" s="58"/>
+      <c r="A125" s="59"/>
     </row>
     <row r="126" customHeight="1" spans="1:1">
-      <c r="A126" s="58"/>
+      <c r="A126" s="59"/>
     </row>
     <row r="127" customHeight="1" spans="1:1">
-      <c r="A127" s="58"/>
+      <c r="A127" s="59"/>
     </row>
     <row r="128" customHeight="1" spans="1:1">
-      <c r="A128" s="58"/>
+      <c r="A128" s="59"/>
     </row>
     <row r="129" customHeight="1" spans="1:1">
-      <c r="A129" s="58"/>
+      <c r="A129" s="59"/>
     </row>
     <row r="130" customHeight="1" spans="1:1">
-      <c r="A130" s="58"/>
+      <c r="A130" s="59"/>
     </row>
     <row r="131" customHeight="1" spans="1:1">
-      <c r="A131" s="58"/>
+      <c r="A131" s="59"/>
     </row>
     <row r="132" customHeight="1" spans="1:1">
-      <c r="A132" s="58"/>
+      <c r="A132" s="59"/>
     </row>
     <row r="133" customHeight="1" spans="1:1">
-      <c r="A133" s="58"/>
+      <c r="A133" s="59"/>
     </row>
     <row r="134" customHeight="1" spans="1:1">
-      <c r="A134" s="58"/>
+      <c r="A134" s="59"/>
     </row>
     <row r="135" customHeight="1" spans="1:1">
-      <c r="A135" s="58"/>
+      <c r="A135" s="59"/>
     </row>
     <row r="136" customHeight="1" spans="1:1">
-      <c r="A136" s="58"/>
+      <c r="A136" s="59"/>
     </row>
     <row r="137" customHeight="1" spans="1:1">
-      <c r="A137" s="58"/>
+      <c r="A137" s="59"/>
     </row>
     <row r="138" customHeight="1" spans="1:1">
-      <c r="A138" s="58"/>
+      <c r="A138" s="59"/>
     </row>
     <row r="139" customHeight="1" spans="1:1">
-      <c r="A139" s="58"/>
+      <c r="A139" s="59"/>
     </row>
     <row r="140" customHeight="1" spans="1:1">
-      <c r="A140" s="58"/>
+      <c r="A140" s="59"/>
     </row>
     <row r="141" customHeight="1" spans="1:1">
-      <c r="A141" s="58"/>
+      <c r="A141" s="59"/>
     </row>
     <row r="142" customHeight="1" spans="1:1">
-      <c r="A142" s="58"/>
+      <c r="A142" s="59"/>
     </row>
     <row r="143" customHeight="1" spans="1:1">
-      <c r="A143" s="58"/>
+      <c r="A143" s="59"/>
     </row>
     <row r="144" customHeight="1" spans="1:1">
-      <c r="A144" s="58"/>
+      <c r="A144" s="59"/>
     </row>
     <row r="145" customHeight="1" spans="1:1">
-      <c r="A145" s="58"/>
+      <c r="A145" s="59"/>
     </row>
     <row r="146" customHeight="1" spans="1:1">
-      <c r="A146" s="58"/>
+      <c r="A146" s="59"/>
     </row>
     <row r="147" customHeight="1" spans="1:1">
-      <c r="A147" s="58"/>
+      <c r="A147" s="59"/>
     </row>
     <row r="148" customHeight="1" spans="1:1">
-      <c r="A148" s="58"/>
+      <c r="A148" s="59"/>
     </row>
     <row r="149" customHeight="1" spans="1:1">
-      <c r="A149" s="58"/>
+      <c r="A149" s="59"/>
     </row>
     <row r="150" customHeight="1" spans="1:1">
-      <c r="A150" s="58"/>
+      <c r="A150" s="59"/>
     </row>
     <row r="151" customHeight="1" spans="1:1">
-      <c r="A151" s="58"/>
+      <c r="A151" s="59"/>
     </row>
     <row r="152" customHeight="1" spans="1:1">
-      <c r="A152" s="58"/>
+      <c r="A152" s="59"/>
     </row>
     <row r="153" customHeight="1" spans="1:1">
-      <c r="A153" s="58"/>
+      <c r="A153" s="59"/>
     </row>
     <row r="154" customHeight="1" spans="1:1">
-      <c r="A154" s="58"/>
+      <c r="A154" s="59"/>
     </row>
     <row r="155" customHeight="1" spans="1:1">
-      <c r="A155" s="58"/>
+      <c r="A155" s="59"/>
     </row>
     <row r="156" customHeight="1" spans="1:1">
-      <c r="A156" s="58"/>
+      <c r="A156" s="59"/>
     </row>
     <row r="157" customHeight="1" spans="1:1">
-      <c r="A157" s="58"/>
+      <c r="A157" s="59"/>
     </row>
     <row r="158" customHeight="1" spans="1:1">
-      <c r="A158" s="58"/>
+      <c r="A158" s="59"/>
     </row>
     <row r="159" customHeight="1" spans="1:1">
-      <c r="A159" s="58"/>
+      <c r="A159" s="59"/>
     </row>
     <row r="160" customHeight="1" spans="1:1">
-      <c r="A160" s="58"/>
+      <c r="A160" s="59"/>
     </row>
     <row r="161" customHeight="1" spans="1:1">
-      <c r="A161" s="58"/>
+      <c r="A161" s="59"/>
     </row>
     <row r="162" customHeight="1" spans="1:1">
-      <c r="A162" s="58"/>
+      <c r="A162" s="59"/>
     </row>
     <row r="163" customHeight="1" spans="1:1">
-      <c r="A163" s="58"/>
+      <c r="A163" s="59"/>
     </row>
     <row r="164" customHeight="1" spans="1:1">
-      <c r="A164" s="58"/>
+      <c r="A164" s="59"/>
     </row>
     <row r="165" customHeight="1" spans="1:1">
-      <c r="A165" s="58"/>
+      <c r="A165" s="59"/>
     </row>
     <row r="166" customHeight="1" spans="1:1">
-      <c r="A166" s="58"/>
+      <c r="A166" s="59"/>
     </row>
     <row r="167" customHeight="1" spans="1:1">
-      <c r="A167" s="58"/>
+      <c r="A167" s="59"/>
     </row>
     <row r="168" customHeight="1" spans="1:1">
-      <c r="A168" s="58"/>
+      <c r="A168" s="59"/>
     </row>
     <row r="169" customHeight="1" spans="1:1">
-      <c r="A169" s="58"/>
+      <c r="A169" s="59"/>
     </row>
     <row r="170" customHeight="1" spans="1:1">
-      <c r="A170" s="58"/>
+      <c r="A170" s="59"/>
     </row>
     <row r="171" customHeight="1" spans="1:1">
-      <c r="A171" s="58"/>
+      <c r="A171" s="59"/>
     </row>
     <row r="172" customHeight="1" spans="1:1">
-      <c r="A172" s="58"/>
+      <c r="A172" s="59"/>
     </row>
     <row r="173" customHeight="1" spans="1:1">
-      <c r="A173" s="58"/>
+      <c r="A173" s="59"/>
     </row>
     <row r="174" customHeight="1" spans="1:1">
-      <c r="A174" s="58"/>
+      <c r="A174" s="59"/>
     </row>
     <row r="175" customHeight="1" spans="1:1">
-      <c r="A175" s="58"/>
+      <c r="A175" s="59"/>
     </row>
     <row r="176" customHeight="1" spans="1:1">
-      <c r="A176" s="58"/>
+      <c r="A176" s="59"/>
     </row>
     <row r="177" customHeight="1" spans="1:1">
-      <c r="A177" s="58"/>
+      <c r="A177" s="59"/>
     </row>
     <row r="178" customHeight="1" spans="1:1">
-      <c r="A178" s="58"/>
+      <c r="A178" s="59"/>
     </row>
     <row r="179" customHeight="1" spans="1:1">
-      <c r="A179" s="58"/>
+      <c r="A179" s="59"/>
     </row>
     <row r="180" customHeight="1" spans="1:1">
-      <c r="A180" s="58"/>
+      <c r="A180" s="59"/>
     </row>
     <row r="181" customHeight="1" spans="1:1">
-      <c r="A181" s="58"/>
+      <c r="A181" s="59"/>
     </row>
     <row r="182" customHeight="1" spans="1:1">
-      <c r="A182" s="58"/>
+      <c r="A182" s="59"/>
     </row>
     <row r="183" customHeight="1" spans="1:1">
-      <c r="A183" s="58"/>
+      <c r="A183" s="59"/>
     </row>
     <row r="184" customHeight="1" spans="1:1">
-      <c r="A184" s="58"/>
+      <c r="A184" s="59"/>
     </row>
     <row r="185" customHeight="1" spans="1:1">
-      <c r="A185" s="58"/>
+      <c r="A185" s="59"/>
     </row>
     <row r="186" customHeight="1" spans="1:1">
-      <c r="A186" s="58"/>
+      <c r="A186" s="59"/>
     </row>
     <row r="187" customHeight="1" spans="1:1">
-      <c r="A187" s="58"/>
+      <c r="A187" s="59"/>
     </row>
     <row r="188" customHeight="1" spans="1:1">
-      <c r="A188" s="58"/>
+      <c r="A188" s="59"/>
     </row>
     <row r="189" customHeight="1" spans="1:1">
-      <c r="A189" s="58"/>
+      <c r="A189" s="59"/>
     </row>
     <row r="190" customHeight="1" spans="1:1">
-      <c r="A190" s="58"/>
+      <c r="A190" s="59"/>
     </row>
     <row r="191" customHeight="1" spans="1:1">
-      <c r="A191" s="58"/>
+      <c r="A191" s="59"/>
     </row>
     <row r="192" customHeight="1" spans="1:1">
-      <c r="A192" s="58"/>
+      <c r="A192" s="59"/>
     </row>
     <row r="193" customHeight="1" spans="1:1">
-      <c r="A193" s="58"/>
+      <c r="A193" s="59"/>
     </row>
     <row r="194" customHeight="1" spans="1:1">
-      <c r="A194" s="58"/>
+      <c r="A194" s="59"/>
     </row>
     <row r="195" customHeight="1" spans="1:1">
-      <c r="A195" s="58"/>
+      <c r="A195" s="59"/>
     </row>
     <row r="196" customHeight="1" spans="1:1">
-      <c r="A196" s="58"/>
+      <c r="A196" s="59"/>
     </row>
     <row r="197" customHeight="1" spans="1:1">
-      <c r="A197" s="58"/>
+      <c r="A197" s="59"/>
     </row>
     <row r="198" customHeight="1" spans="1:1">
-      <c r="A198" s="58"/>
+      <c r="A198" s="59"/>
     </row>
     <row r="199" customHeight="1" spans="1:1">
-      <c r="A199" s="58"/>
+      <c r="A199" s="59"/>
     </row>
     <row r="200" customHeight="1" spans="1:1">
-      <c r="A200" s="58"/>
+      <c r="A200" s="59"/>
     </row>
     <row r="201" customHeight="1" spans="1:1">
-      <c r="A201" s="58"/>
+      <c r="A201" s="59"/>
     </row>
     <row r="202" customHeight="1" spans="1:1">
-      <c r="A202" s="58"/>
+      <c r="A202" s="59"/>
     </row>
     <row r="203" customHeight="1" spans="1:1">
-      <c r="A203" s="58"/>
+      <c r="A203" s="59"/>
     </row>
     <row r="204" customHeight="1" spans="1:1">
-      <c r="A204" s="58"/>
+      <c r="A204" s="59"/>
     </row>
     <row r="205" customHeight="1" spans="1:1">
-      <c r="A205" s="58"/>
+      <c r="A205" s="59"/>
     </row>
     <row r="206" customHeight="1" spans="1:1">
-      <c r="A206" s="58"/>
+      <c r="A206" s="59"/>
     </row>
     <row r="207" customHeight="1" spans="1:1">
-      <c r="A207" s="58"/>
+      <c r="A207" s="59"/>
     </row>
     <row r="208" customHeight="1" spans="1:1">
-      <c r="A208" s="58"/>
+      <c r="A208" s="59"/>
     </row>
     <row r="209" customHeight="1" spans="1:1">
-      <c r="A209" s="58"/>
+      <c r="A209" s="59"/>
     </row>
     <row r="210" customHeight="1" spans="1:1">
-      <c r="A210" s="58"/>
+      <c r="A210" s="59"/>
     </row>
     <row r="211" customHeight="1" spans="1:1">
-      <c r="A211" s="58"/>
+      <c r="A211" s="59"/>
     </row>
     <row r="212" customHeight="1" spans="1:1">
-      <c r="A212" s="58"/>
+      <c r="A212" s="59"/>
     </row>
     <row r="213" customHeight="1" spans="1:1">
-      <c r="A213" s="58"/>
+      <c r="A213" s="59"/>
     </row>
     <row r="214" customHeight="1" spans="1:1">
-      <c r="A214" s="58"/>
+      <c r="A214" s="59"/>
     </row>
     <row r="215" customHeight="1" spans="1:1">
-      <c r="A215" s="58"/>
+      <c r="A215" s="59"/>
     </row>
     <row r="216" customHeight="1" spans="1:1">
-      <c r="A216" s="58"/>
+      <c r="A216" s="59"/>
     </row>
     <row r="217" customHeight="1" spans="1:1">
-      <c r="A217" s="58"/>
+      <c r="A217" s="59"/>
     </row>
     <row r="218" customHeight="1" spans="1:1">
-      <c r="A218" s="58"/>
+      <c r="A218" s="59"/>
     </row>
     <row r="219" customHeight="1" spans="1:1">
-      <c r="A219" s="58"/>
+      <c r="A219" s="59"/>
     </row>
     <row r="220" customHeight="1" spans="1:1">
-      <c r="A220" s="58"/>
+      <c r="A220" s="59"/>
     </row>
     <row r="221" customHeight="1" spans="1:1">
-      <c r="A221" s="58"/>
+      <c r="A221" s="59"/>
     </row>
     <row r="222" customHeight="1" spans="1:1">
-      <c r="A222" s="58"/>
+      <c r="A222" s="59"/>
     </row>
     <row r="223" customHeight="1" spans="1:1">
-      <c r="A223" s="58"/>
+      <c r="A223" s="59"/>
     </row>
     <row r="224" customHeight="1" spans="1:1">
-      <c r="A224" s="58"/>
+      <c r="A224" s="59"/>
     </row>
     <row r="225" customHeight="1" spans="1:1">
-      <c r="A225" s="58"/>
+      <c r="A225" s="59"/>
     </row>
     <row r="226" customHeight="1" spans="1:1">
-      <c r="A226" s="58"/>
+      <c r="A226" s="59"/>
     </row>
     <row r="227" customHeight="1" spans="1:1">
-      <c r="A227" s="58"/>
+      <c r="A227" s="59"/>
     </row>
     <row r="228" customHeight="1" spans="1:1">
-      <c r="A228" s="58"/>
+      <c r="A228" s="59"/>
     </row>
     <row r="229" customHeight="1" spans="1:1">
-      <c r="A229" s="58"/>
+      <c r="A229" s="59"/>
     </row>
     <row r="230" customHeight="1" spans="1:1">
-      <c r="A230" s="58"/>
+      <c r="A230" s="59"/>
     </row>
     <row r="231" customHeight="1" spans="1:1">
-      <c r="A231" s="58"/>
+      <c r="A231" s="59"/>
     </row>
     <row r="232" customHeight="1" spans="1:1">
-      <c r="A232" s="58"/>
+      <c r="A232" s="59"/>
     </row>
     <row r="233" customHeight="1" spans="1:1">
-      <c r="A233" s="58"/>
+      <c r="A233" s="59"/>
     </row>
     <row r="234" customHeight="1" spans="1:1">
-      <c r="A234" s="58"/>
+      <c r="A234" s="59"/>
     </row>
     <row r="235" customHeight="1" spans="1:1">
-      <c r="A235" s="58"/>
+      <c r="A235" s="59"/>
     </row>
     <row r="236" customHeight="1" spans="1:1">
-      <c r="A236" s="58"/>
+      <c r="A236" s="59"/>
     </row>
     <row r="237" customHeight="1" spans="1:1">
-      <c r="A237" s="58"/>
+      <c r="A237" s="59"/>
     </row>
     <row r="238" customHeight="1" spans="1:1">
-      <c r="A238" s="58"/>
+      <c r="A238" s="59"/>
     </row>
     <row r="239" customHeight="1" spans="1:1">
-      <c r="A239" s="58"/>
+      <c r="A239" s="59"/>
     </row>
     <row r="240" customHeight="1" spans="1:1">
-      <c r="A240" s="58"/>
+      <c r="A240" s="59"/>
     </row>
     <row r="241" customHeight="1" spans="1:1">
-      <c r="A241" s="58"/>
+      <c r="A241" s="59"/>
     </row>
     <row r="242" customHeight="1" spans="1:1">
-      <c r="A242" s="58"/>
+      <c r="A242" s="59"/>
     </row>
     <row r="243" customHeight="1" spans="1:1">
-      <c r="A243" s="58"/>
+      <c r="A243" s="59"/>
     </row>
     <row r="244" customHeight="1" spans="1:1">
-      <c r="A244" s="58"/>
+      <c r="A244" s="59"/>
     </row>
     <row r="245" customHeight="1" spans="1:1">
-      <c r="A245" s="58"/>
+      <c r="A245" s="59"/>
     </row>
     <row r="246" customHeight="1" spans="1:1">
-      <c r="A246" s="58"/>
+      <c r="A246" s="59"/>
     </row>
     <row r="247" customHeight="1" spans="1:1">
-      <c r="A247" s="58"/>
+      <c r="A247" s="59"/>
     </row>
     <row r="248" customHeight="1" spans="1:1">
-      <c r="A248" s="58"/>
+      <c r="A248" s="59"/>
     </row>
     <row r="249" customHeight="1" spans="1:1">
-      <c r="A249" s="58"/>
+      <c r="A249" s="59"/>
     </row>
     <row r="250" customHeight="1" spans="1:1">
-      <c r="A250" s="58"/>
+      <c r="A250" s="59"/>
     </row>
     <row r="251" customHeight="1" spans="1:1">
-      <c r="A251" s="58"/>
+      <c r="A251" s="59"/>
     </row>
     <row r="252" customHeight="1" spans="1:1">
-      <c r="A252" s="58"/>
+      <c r="A252" s="59"/>
     </row>
     <row r="253" customHeight="1" spans="1:1">
-      <c r="A253" s="58"/>
+      <c r="A253" s="59"/>
     </row>
     <row r="254" customHeight="1" spans="1:1">
-      <c r="A254" s="58"/>
+      <c r="A254" s="59"/>
     </row>
     <row r="255" customHeight="1" spans="1:1">
-      <c r="A255" s="58"/>
+      <c r="A255" s="59"/>
     </row>
     <row r="256" customHeight="1" spans="1:1">
-      <c r="A256" s="58"/>
+      <c r="A256" s="59"/>
     </row>
     <row r="257" customHeight="1" spans="1:1">
-      <c r="A257" s="58"/>
+      <c r="A257" s="59"/>
     </row>
     <row r="258" customHeight="1" spans="1:1">
-      <c r="A258" s="58"/>
+      <c r="A258" s="59"/>
     </row>
     <row r="259" customHeight="1" spans="1:1">
-      <c r="A259" s="58"/>
+      <c r="A259" s="59"/>
     </row>
     <row r="260" customHeight="1" spans="1:1">
-      <c r="A260" s="58"/>
+      <c r="A260" s="59"/>
     </row>
     <row r="261" customHeight="1" spans="1:1">
-      <c r="A261" s="58"/>
+      <c r="A261" s="59"/>
     </row>
     <row r="262" customHeight="1" spans="1:1">
-      <c r="A262" s="58"/>
+      <c r="A262" s="59"/>
     </row>
     <row r="263" customHeight="1" spans="1:1">
-      <c r="A263" s="58"/>
+      <c r="A263" s="59"/>
     </row>
     <row r="264" customHeight="1" spans="1:1">
-      <c r="A264" s="58"/>
+      <c r="A264" s="59"/>
     </row>
     <row r="265" customHeight="1" spans="1:1">
-      <c r="A265" s="58"/>
+      <c r="A265" s="59"/>
     </row>
     <row r="266" customHeight="1" spans="1:1">
-      <c r="A266" s="58"/>
+      <c r="A266" s="59"/>
     </row>
     <row r="267" customHeight="1" spans="1:1">
-      <c r="A267" s="58"/>
+      <c r="A267" s="59"/>
     </row>
     <row r="268" customHeight="1" spans="1:1">
-      <c r="A268" s="58"/>
+      <c r="A268" s="59"/>
     </row>
     <row r="269" customHeight="1" spans="1:1">
-      <c r="A269" s="58"/>
+      <c r="A269" s="59"/>
     </row>
     <row r="270" customHeight="1" spans="1:1">
-      <c r="A270" s="58"/>
+      <c r="A270" s="59"/>
     </row>
     <row r="271" customHeight="1" spans="1:1">
-      <c r="A271" s="58"/>
+      <c r="A271" s="59"/>
     </row>
     <row r="272" customHeight="1" spans="1:1">
-      <c r="A272" s="58"/>
+      <c r="A272" s="59"/>
     </row>
     <row r="273" customHeight="1" spans="1:1">
-      <c r="A273" s="58"/>
+      <c r="A273" s="59"/>
     </row>
     <row r="274" customHeight="1" spans="1:1">
-      <c r="A274" s="58"/>
+      <c r="A274" s="59"/>
     </row>
     <row r="275" customHeight="1" spans="1:1">
-      <c r="A275" s="58"/>
+      <c r="A275" s="59"/>
     </row>
     <row r="276" customHeight="1" spans="1:1">
-      <c r="A276" s="58"/>
+      <c r="A276" s="59"/>
     </row>
     <row r="277" customHeight="1" spans="1:1">
-      <c r="A277" s="58"/>
+      <c r="A277" s="59"/>
     </row>
     <row r="278" customHeight="1" spans="1:1">
-      <c r="A278" s="58"/>
+      <c r="A278" s="59"/>
     </row>
     <row r="279" customHeight="1" spans="1:1">
-      <c r="A279" s="58"/>
+      <c r="A279" s="59"/>
     </row>
     <row r="280" customHeight="1" spans="1:1">
-      <c r="A280" s="58"/>
+      <c r="A280" s="59"/>
     </row>
     <row r="281" customHeight="1" spans="1:1">
-      <c r="A281" s="58"/>
+      <c r="A281" s="59"/>
     </row>
     <row r="282" customHeight="1" spans="1:1">
-      <c r="A282" s="58"/>
+      <c r="A282" s="59"/>
     </row>
     <row r="283" customHeight="1" spans="1:1">
-      <c r="A283" s="58"/>
+      <c r="A283" s="59"/>
     </row>
     <row r="284" customHeight="1" spans="1:1">
-      <c r="A284" s="58"/>
+      <c r="A284" s="59"/>
     </row>
     <row r="285" customHeight="1" spans="1:1">
-      <c r="A285" s="58"/>
+      <c r="A285" s="59"/>
     </row>
     <row r="286" customHeight="1" spans="1:1">
-      <c r="A286" s="58"/>
+      <c r="A286" s="59"/>
     </row>
     <row r="287" customHeight="1" spans="1:1">
-      <c r="A287" s="58"/>
+      <c r="A287" s="59"/>
     </row>
     <row r="288" customHeight="1" spans="1:1">
-      <c r="A288" s="58"/>
+      <c r="A288" s="59"/>
     </row>
     <row r="289" customHeight="1" spans="1:1">
-      <c r="A289" s="58"/>
+      <c r="A289" s="59"/>
     </row>
     <row r="290" customHeight="1" spans="1:1">
-      <c r="A290" s="58"/>
+      <c r="A290" s="59"/>
     </row>
     <row r="291" customHeight="1" spans="1:1">
-      <c r="A291" s="58"/>
+      <c r="A291" s="59"/>
     </row>
     <row r="292" customHeight="1" spans="1:1">
-      <c r="A292" s="58"/>
+      <c r="A292" s="59"/>
     </row>
     <row r="293" customHeight="1" spans="1:1">
-      <c r="A293" s="58"/>
+      <c r="A293" s="59"/>
     </row>
     <row r="294" customHeight="1" spans="1:1">
-      <c r="A294" s="58"/>
+      <c r="A294" s="59"/>
     </row>
     <row r="295" customHeight="1" spans="1:1">
-      <c r="A295" s="58"/>
+      <c r="A295" s="59"/>
     </row>
     <row r="296" customHeight="1" spans="1:1">
-      <c r="A296" s="58"/>
+      <c r="A296" s="59"/>
     </row>
     <row r="297" customHeight="1" spans="1:1">
-      <c r="A297" s="58"/>
+      <c r="A297" s="59"/>
     </row>
     <row r="298" customHeight="1" spans="1:1">
-      <c r="A298" s="58"/>
+      <c r="A298" s="59"/>
     </row>
     <row r="299" customHeight="1" spans="1:1">
-      <c r="A299" s="58"/>
+      <c r="A299" s="59"/>
     </row>
     <row r="300" customHeight="1" spans="1:1">
-      <c r="A300" s="58"/>
+      <c r="A300" s="59"/>
     </row>
     <row r="301" customHeight="1" spans="1:1">
-      <c r="A301" s="58"/>
+      <c r="A301" s="59"/>
     </row>
     <row r="302" customHeight="1" spans="1:1">
-      <c r="A302" s="58"/>
+      <c r="A302" s="59"/>
     </row>
     <row r="303" customHeight="1" spans="1:1">
-      <c r="A303" s="58"/>
+      <c r="A303" s="59"/>
     </row>
     <row r="304" customHeight="1" spans="1:1">
-      <c r="A304" s="58"/>
+      <c r="A304" s="59"/>
     </row>
     <row r="305" customHeight="1" spans="1:1">
-      <c r="A305" s="58"/>
+      <c r="A305" s="59"/>
     </row>
     <row r="306" customHeight="1" spans="1:1">
-      <c r="A306" s="58"/>
+      <c r="A306" s="59"/>
     </row>
     <row r="307" customHeight="1" spans="1:1">
-      <c r="A307" s="58"/>
+      <c r="A307" s="59"/>
     </row>
     <row r="308" customHeight="1" spans="1:1">
-      <c r="A308" s="58"/>
+      <c r="A308" s="59"/>
     </row>
     <row r="309" customHeight="1" spans="1:1">
-      <c r="A309" s="58"/>
+      <c r="A309" s="59"/>
     </row>
     <row r="310" customHeight="1" spans="1:1">
-      <c r="A310" s="58"/>
+      <c r="A310" s="59"/>
     </row>
     <row r="311" customHeight="1" spans="1:1">
-      <c r="A311" s="58"/>
+      <c r="A311" s="59"/>
     </row>
     <row r="312" customHeight="1" spans="1:1">
-      <c r="A312" s="58"/>
+      <c r="A312" s="59"/>
     </row>
     <row r="313" customHeight="1" spans="1:1">
-      <c r="A313" s="58"/>
+      <c r="A313" s="59"/>
     </row>
     <row r="314" customHeight="1" spans="1:1">
-      <c r="A314" s="58"/>
+      <c r="A314" s="59"/>
     </row>
     <row r="315" customHeight="1" spans="1:1">
-      <c r="A315" s="58"/>
+      <c r="A315" s="59"/>
     </row>
     <row r="316" customHeight="1" spans="1:1">
-      <c r="A316" s="58"/>
+      <c r="A316" s="59"/>
     </row>
     <row r="317" customHeight="1" spans="1:1">
-      <c r="A317" s="58"/>
+      <c r="A317" s="59"/>
     </row>
     <row r="318" customHeight="1" spans="1:1">
-      <c r="A318" s="58"/>
+      <c r="A318" s="59"/>
     </row>
     <row r="319" customHeight="1" spans="1:1">
-      <c r="A319" s="58"/>
+      <c r="A319" s="59"/>
     </row>
     <row r="320" customHeight="1" spans="1:1">
-      <c r="A320" s="58"/>
+      <c r="A320" s="59"/>
     </row>
     <row r="321" customHeight="1" spans="1:1">
-      <c r="A321" s="58"/>
+      <c r="A321" s="59"/>
     </row>
     <row r="322" customHeight="1" spans="1:1">
-      <c r="A322" s="58"/>
+      <c r="A322" s="59"/>
     </row>
     <row r="323" customHeight="1" spans="1:1">
-      <c r="A323" s="58"/>
+      <c r="A323" s="59"/>
     </row>
     <row r="324" customHeight="1" spans="1:1">
-      <c r="A324" s="58"/>
+      <c r="A324" s="59"/>
     </row>
     <row r="325" customHeight="1" spans="1:1">
-      <c r="A325" s="58"/>
+      <c r="A325" s="59"/>
     </row>
     <row r="326" customHeight="1" spans="1:1">
-      <c r="A326" s="58"/>
+      <c r="A326" s="59"/>
     </row>
     <row r="327" customHeight="1" spans="1:1">
-      <c r="A327" s="58"/>
+      <c r="A327" s="59"/>
     </row>
     <row r="328" customHeight="1" spans="1:1">
-      <c r="A328" s="58"/>
+      <c r="A328" s="59"/>
     </row>
     <row r="329" customHeight="1" spans="1:1">
-      <c r="A329" s="58"/>
+      <c r="A329" s="59"/>
     </row>
     <row r="330" customHeight="1" spans="1:1">
-      <c r="A330" s="58"/>
+      <c r="A330" s="59"/>
     </row>
     <row r="331" customHeight="1" spans="1:1">
-      <c r="A331" s="58"/>
+      <c r="A331" s="59"/>
     </row>
     <row r="332" customHeight="1" spans="1:1">
-      <c r="A332" s="58"/>
+      <c r="A332" s="59"/>
     </row>
     <row r="333" customHeight="1" spans="1:1">
-      <c r="A333" s="58"/>
+      <c r="A333" s="59"/>
     </row>
     <row r="334" customHeight="1" spans="1:1">
-      <c r="A334" s="58"/>
+      <c r="A334" s="59"/>
     </row>
     <row r="335" customHeight="1" spans="1:1">
-      <c r="A335" s="58"/>
+      <c r="A335" s="59"/>
     </row>
     <row r="336" customHeight="1" spans="1:1">
-      <c r="A336" s="58"/>
+      <c r="A336" s="59"/>
     </row>
     <row r="337" customHeight="1" spans="1:1">
-      <c r="A337" s="58"/>
+      <c r="A337" s="59"/>
     </row>
     <row r="338" customHeight="1" spans="1:1">
-      <c r="A338" s="58"/>
+      <c r="A338" s="59"/>
     </row>
     <row r="339" customHeight="1" spans="1:1">
-      <c r="A339" s="58"/>
+      <c r="A339" s="59"/>
     </row>
     <row r="340" customHeight="1" spans="1:1">
-      <c r="A340" s="58"/>
+      <c r="A340" s="59"/>
     </row>
     <row r="341" customHeight="1" spans="1:1">
-      <c r="A341" s="58"/>
+      <c r="A341" s="59"/>
     </row>
     <row r="342" customHeight="1" spans="1:1">
-      <c r="A342" s="58"/>
+      <c r="A342" s="59"/>
     </row>
     <row r="343" customHeight="1" spans="1:1">
-      <c r="A343" s="58"/>
+      <c r="A343" s="59"/>
     </row>
     <row r="344" customHeight="1" spans="1:1">
-      <c r="A344" s="58"/>
+      <c r="A344" s="59"/>
     </row>
     <row r="345" customHeight="1" spans="1:1">
-      <c r="A345" s="58"/>
+      <c r="A345" s="59"/>
     </row>
     <row r="346" customHeight="1" spans="1:1">
-      <c r="A346" s="58"/>
+      <c r="A346" s="59"/>
     </row>
     <row r="347" customHeight="1" spans="1:1">
-      <c r="A347" s="58"/>
+      <c r="A347" s="59"/>
     </row>
     <row r="348" customHeight="1" spans="1:1">
-      <c r="A348" s="58"/>
+      <c r="A348" s="59"/>
     </row>
     <row r="349" customHeight="1" spans="1:1">
-      <c r="A349" s="58"/>
+      <c r="A349" s="59"/>
     </row>
     <row r="350" customHeight="1" spans="1:1">
-      <c r="A350" s="58"/>
+      <c r="A350" s="59"/>
     </row>
     <row r="351" customHeight="1" spans="1:1">
-      <c r="A351" s="58"/>
+      <c r="A351" s="59"/>
     </row>
     <row r="352" customHeight="1" spans="1:1">
-      <c r="A352" s="58"/>
+      <c r="A352" s="59"/>
     </row>
     <row r="353" customHeight="1" spans="1:1">
-      <c r="A353" s="58"/>
+      <c r="A353" s="59"/>
     </row>
     <row r="354" customHeight="1" spans="1:1">
-      <c r="A354" s="58"/>
+      <c r="A354" s="59"/>
     </row>
     <row r="355" customHeight="1" spans="1:1">
-      <c r="A355" s="58"/>
+      <c r="A355" s="59"/>
     </row>
     <row r="356" customHeight="1" spans="1:1">
-      <c r="A356" s="58"/>
+      <c r="A356" s="59"/>
     </row>
     <row r="357" customHeight="1" spans="1:1">
-      <c r="A357" s="58"/>
+      <c r="A357" s="59"/>
     </row>
     <row r="358" customHeight="1" spans="1:1">
-      <c r="A358" s="58"/>
+      <c r="A358" s="59"/>
     </row>
     <row r="359" customHeight="1" spans="1:1">
-      <c r="A359" s="58"/>
+      <c r="A359" s="59"/>
     </row>
     <row r="360" customHeight="1" spans="1:1">
-      <c r="A360" s="58"/>
+      <c r="A360" s="59"/>
     </row>
     <row r="361" customHeight="1" spans="1:1">
-      <c r="A361" s="58"/>
+      <c r="A361" s="59"/>
     </row>
     <row r="362" customHeight="1" spans="1:1">
-      <c r="A362" s="58"/>
+      <c r="A362" s="59"/>
     </row>
     <row r="363" customHeight="1" spans="1:1">
-      <c r="A363" s="58"/>
+      <c r="A363" s="59"/>
     </row>
     <row r="364" customHeight="1" spans="1:1">
-      <c r="A364" s="58"/>
+      <c r="A364" s="59"/>
     </row>
     <row r="365" customHeight="1" spans="1:1">
-      <c r="A365" s="58"/>
+      <c r="A365" s="59"/>
     </row>
     <row r="366" customHeight="1" spans="1:1">
-      <c r="A366" s="58"/>
+      <c r="A366" s="59"/>
     </row>
     <row r="367" customHeight="1" spans="1:1">
-      <c r="A367" s="58"/>
+      <c r="A367" s="59"/>
     </row>
     <row r="368" customHeight="1" spans="1:1">
-      <c r="A368" s="58"/>
+      <c r="A368" s="59"/>
     </row>
     <row r="369" customHeight="1" spans="1:1">
-      <c r="A369" s="58"/>
+      <c r="A369" s="59"/>
     </row>
     <row r="370" customHeight="1" spans="1:1">
-      <c r="A370" s="58"/>
+      <c r="A370" s="59"/>
     </row>
     <row r="371" customHeight="1" spans="1:1">
-      <c r="A371" s="58"/>
+      <c r="A371" s="59"/>
     </row>
     <row r="372" customHeight="1" spans="1:1">
-      <c r="A372" s="58"/>
+      <c r="A372" s="59"/>
     </row>
     <row r="373" customHeight="1" spans="1:1">
-      <c r="A373" s="58"/>
+      <c r="A373" s="59"/>
     </row>
     <row r="374" customHeight="1" spans="1:1">
-      <c r="A374" s="58"/>
+      <c r="A374" s="59"/>
     </row>
     <row r="375" customHeight="1" spans="1:1">
-      <c r="A375" s="58"/>
+      <c r="A375" s="59"/>
     </row>
     <row r="376" customHeight="1" spans="1:1">
-      <c r="A376" s="58"/>
+      <c r="A376" s="59"/>
     </row>
     <row r="377" customHeight="1" spans="1:1">
-      <c r="A377" s="58"/>
+      <c r="A377" s="59"/>
     </row>
     <row r="378" customHeight="1" spans="1:1">
-      <c r="A378" s="58"/>
+      <c r="A378" s="59"/>
     </row>
     <row r="379" customHeight="1" spans="1:1">
-      <c r="A379" s="58"/>
+      <c r="A379" s="59"/>
     </row>
     <row r="380" customHeight="1" spans="1:1">
-      <c r="A380" s="58"/>
+      <c r="A380" s="59"/>
     </row>
     <row r="381" customHeight="1" spans="1:1">
-      <c r="A381" s="58"/>
+      <c r="A381" s="59"/>
     </row>
     <row r="382" customHeight="1" spans="1:1">
-      <c r="A382" s="58"/>
+      <c r="A382" s="59"/>
     </row>
     <row r="383" customHeight="1" spans="1:1">
-      <c r="A383" s="58"/>
+      <c r="A383" s="59"/>
     </row>
     <row r="384" customHeight="1" spans="1:1">
-      <c r="A384" s="58"/>
+      <c r="A384" s="59"/>
     </row>
     <row r="385" customHeight="1" spans="1:1">
-      <c r="A385" s="58"/>
+      <c r="A385" s="59"/>
     </row>
     <row r="386" customHeight="1" spans="1:1">
-      <c r="A386" s="58"/>
+      <c r="A386" s="59"/>
     </row>
     <row r="387" customHeight="1" spans="1:1">
-      <c r="A387" s="58"/>
+      <c r="A387" s="59"/>
     </row>
     <row r="388" customHeight="1" spans="1:1">
-      <c r="A388" s="58"/>
+      <c r="A388" s="59"/>
     </row>
     <row r="389" customHeight="1" spans="1:1">
-      <c r="A389" s="58"/>
+      <c r="A389" s="59"/>
     </row>
     <row r="390" customHeight="1" spans="1:1">
-      <c r="A390" s="58"/>
+      <c r="A390" s="59"/>
     </row>
     <row r="391" customHeight="1" spans="1:1">
-      <c r="A391" s="58"/>
+      <c r="A391" s="59"/>
     </row>
     <row r="392" customHeight="1" spans="1:1">
-      <c r="A392" s="58"/>
+      <c r="A392" s="59"/>
     </row>
     <row r="393" customHeight="1" spans="1:1">
-      <c r="A393" s="58"/>
+      <c r="A393" s="59"/>
     </row>
     <row r="394" customHeight="1" spans="1:1">
-      <c r="A394" s="58"/>
+      <c r="A394" s="59"/>
     </row>
     <row r="395" customHeight="1" spans="1:1">
-      <c r="A395" s="58"/>
+      <c r="A395" s="59"/>
     </row>
     <row r="396" customHeight="1" spans="1:1">
-      <c r="A396" s="58"/>
+      <c r="A396" s="59"/>
     </row>
     <row r="397" customHeight="1" spans="1:1">
-      <c r="A397" s="58"/>
+      <c r="A397" s="59"/>
     </row>
     <row r="398" customHeight="1" spans="1:1">
-      <c r="A398" s="58"/>
+      <c r="A398" s="59"/>
     </row>
     <row r="399" customHeight="1" spans="1:1">
-      <c r="A399" s="58"/>
+      <c r="A399" s="59"/>
     </row>
     <row r="400" customHeight="1" spans="1:1">
-      <c r="A400" s="58"/>
+      <c r="A400" s="59"/>
     </row>
     <row r="401" customHeight="1" spans="1:1">
-      <c r="A401" s="58"/>
+      <c r="A401" s="59"/>
     </row>
     <row r="402" customHeight="1" spans="1:1">
-      <c r="A402" s="58"/>
+      <c r="A402" s="59"/>
     </row>
     <row r="403" customHeight="1" spans="1:1">
-      <c r="A403" s="58"/>
+      <c r="A403" s="59"/>
     </row>
     <row r="404" customHeight="1" spans="1:1">
-      <c r="A404" s="58"/>
+      <c r="A404" s="59"/>
     </row>
     <row r="405" customHeight="1" spans="1:1">
-      <c r="A405" s="58"/>
+      <c r="A405" s="59"/>
     </row>
     <row r="406" customHeight="1" spans="1:1">
-      <c r="A406" s="58"/>
+      <c r="A406" s="59"/>
     </row>
     <row r="407" customHeight="1" spans="1:1">
-      <c r="A407" s="58"/>
+      <c r="A407" s="59"/>
     </row>
     <row r="408" customHeight="1" spans="1:1">
-      <c r="A408" s="58"/>
+      <c r="A408" s="59"/>
     </row>
     <row r="409" customHeight="1" spans="1:1">
-      <c r="A409" s="58"/>
+      <c r="A409" s="59"/>
     </row>
     <row r="410" customHeight="1" spans="1:1">
-      <c r="A410" s="58"/>
+      <c r="A410" s="59"/>
     </row>
     <row r="411" customHeight="1" spans="1:1">
-      <c r="A411" s="58"/>
+      <c r="A411" s="59"/>
     </row>
     <row r="412" customHeight="1" spans="1:1">
-      <c r="A412" s="58"/>
+      <c r="A412" s="59"/>
     </row>
     <row r="413" customHeight="1" spans="1:1">
-      <c r="A413" s="58"/>
+      <c r="A413" s="59"/>
     </row>
     <row r="414" customHeight="1" spans="1:1">
-      <c r="A414" s="58"/>
+      <c r="A414" s="59"/>
     </row>
     <row r="415" customHeight="1" spans="1:1">
-      <c r="A415" s="58"/>
+      <c r="A415" s="59"/>
     </row>
     <row r="416" customHeight="1" spans="1:1">
-      <c r="A416" s="58"/>
+      <c r="A416" s="59"/>
     </row>
     <row r="417" customHeight="1" spans="1:1">
-      <c r="A417" s="58"/>
+      <c r="A417" s="59"/>
     </row>
     <row r="418" customHeight="1" spans="1:1">
-      <c r="A418" s="58"/>
+      <c r="A418" s="59"/>
     </row>
     <row r="419" customHeight="1" spans="1:1">
-      <c r="A419" s="58"/>
+      <c r="A419" s="59"/>
     </row>
     <row r="420" customHeight="1" spans="1:1">
-      <c r="A420" s="58"/>
+      <c r="A420" s="59"/>
     </row>
     <row r="421" customHeight="1" spans="1:1">
-      <c r="A421" s="58"/>
+      <c r="A421" s="59"/>
     </row>
     <row r="422" customHeight="1" spans="1:1">
-      <c r="A422" s="58"/>
+      <c r="A422" s="59"/>
     </row>
     <row r="423" customHeight="1" spans="1:1">
-      <c r="A423" s="58"/>
+      <c r="A423" s="59"/>
     </row>
     <row r="424" customHeight="1" spans="1:1">
-      <c r="A424" s="58"/>
+      <c r="A424" s="59"/>
     </row>
     <row r="425" customHeight="1" spans="1:1">
-      <c r="A425" s="58"/>
+      <c r="A425" s="59"/>
     </row>
     <row r="426" customHeight="1" spans="1:1">
-      <c r="A426" s="58"/>
+      <c r="A426" s="59"/>
     </row>
     <row r="427" customHeight="1" spans="1:1">
-      <c r="A427" s="58"/>
+      <c r="A427" s="59"/>
     </row>
     <row r="428" customHeight="1" spans="1:1">
-      <c r="A428" s="58"/>
+      <c r="A428" s="59"/>
     </row>
     <row r="429" customHeight="1" spans="1:1">
-      <c r="A429" s="58"/>
+      <c r="A429" s="59"/>
     </row>
     <row r="430" customHeight="1" spans="1:1">
-      <c r="A430" s="58"/>
+      <c r="A430" s="59"/>
     </row>
     <row r="431" customHeight="1" spans="1:1">
-      <c r="A431" s="58"/>
+      <c r="A431" s="59"/>
     </row>
     <row r="432" customHeight="1" spans="1:1">
-      <c r="A432" s="58"/>
+      <c r="A432" s="59"/>
     </row>
     <row r="433" customHeight="1" spans="1:1">
-      <c r="A433" s="58"/>
+      <c r="A433" s="59"/>
     </row>
     <row r="434" customHeight="1" spans="1:1">
-      <c r="A434" s="58"/>
+      <c r="A434" s="59"/>
     </row>
     <row r="435" customHeight="1" spans="1:1">
-      <c r="A435" s="58"/>
+      <c r="A435" s="59"/>
     </row>
     <row r="436" customHeight="1" spans="1:1">
-      <c r="A436" s="58"/>
+      <c r="A436" s="59"/>
     </row>
     <row r="437" customHeight="1" spans="1:1">
-      <c r="A437" s="58"/>
+      <c r="A437" s="59"/>
     </row>
     <row r="438" customHeight="1" spans="1:1">
-      <c r="A438" s="58"/>
+      <c r="A438" s="59"/>
     </row>
     <row r="439" customHeight="1" spans="1:1">
-      <c r="A439" s="58"/>
+      <c r="A439" s="59"/>
     </row>
     <row r="440" customHeight="1" spans="1:1">
-      <c r="A440" s="58"/>
+      <c r="A440" s="59"/>
     </row>
     <row r="441" customHeight="1" spans="1:1">
-      <c r="A441" s="58"/>
+      <c r="A441" s="59"/>
     </row>
     <row r="442" customHeight="1" spans="1:1">
-      <c r="A442" s="58"/>
+      <c r="A442" s="59"/>
     </row>
     <row r="443" customHeight="1" spans="1:1">
-      <c r="A443" s="58"/>
+      <c r="A443" s="59"/>
     </row>
     <row r="444" customHeight="1" spans="1:1">
-      <c r="A444" s="58"/>
+      <c r="A444" s="59"/>
     </row>
     <row r="445" customHeight="1" spans="1:1">
-      <c r="A445" s="58"/>
+      <c r="A445" s="59"/>
     </row>
     <row r="446" customHeight="1" spans="1:1">
-      <c r="A446" s="58"/>
+      <c r="A446" s="59"/>
     </row>
     <row r="447" customHeight="1" spans="1:1">
-      <c r="A447" s="58"/>
+      <c r="A447" s="59"/>
     </row>
     <row r="448" customHeight="1" spans="1:1">
-      <c r="A448" s="58"/>
+      <c r="A448" s="59"/>
     </row>
     <row r="449" customHeight="1" spans="1:1">
-      <c r="A449" s="58"/>
+      <c r="A449" s="59"/>
     </row>
     <row r="450" customHeight="1" spans="1:1">
-      <c r="A450" s="58"/>
+      <c r="A450" s="59"/>
     </row>
     <row r="451" customHeight="1" spans="1:1">
-      <c r="A451" s="58"/>
+      <c r="A451" s="59"/>
     </row>
     <row r="452" customHeight="1" spans="1:1">
-      <c r="A452" s="58"/>
+      <c r="A452" s="59"/>
     </row>
     <row r="453" customHeight="1" spans="1:1">
-      <c r="A453" s="58"/>
+      <c r="A453" s="59"/>
     </row>
     <row r="454" customHeight="1" spans="1:1">
-      <c r="A454" s="58"/>
+      <c r="A454" s="59"/>
     </row>
     <row r="455" customHeight="1" spans="1:1">
-      <c r="A455" s="58"/>
+      <c r="A455" s="59"/>
     </row>
     <row r="456" customHeight="1" spans="1:1">
-      <c r="A456" s="58"/>
+      <c r="A456" s="59"/>
     </row>
     <row r="457" customHeight="1" spans="1:1">
-      <c r="A457" s="58"/>
+      <c r="A457" s="59"/>
     </row>
     <row r="458" customHeight="1" spans="1:1">
-      <c r="A458" s="58"/>
+      <c r="A458" s="59"/>
     </row>
     <row r="459" customHeight="1" spans="1:1">
-      <c r="A459" s="58"/>
+      <c r="A459" s="59"/>
     </row>
     <row r="460" customHeight="1" spans="1:1">
-      <c r="A460" s="58"/>
+      <c r="A460" s="59"/>
     </row>
     <row r="461" customHeight="1" spans="1:1">
-      <c r="A461" s="58"/>
+      <c r="A461" s="59"/>
     </row>
     <row r="462" customHeight="1" spans="1:1">
-      <c r="A462" s="58"/>
+      <c r="A462" s="59"/>
     </row>
     <row r="463" customHeight="1" spans="1:1">
-      <c r="A463" s="58"/>
+      <c r="A463" s="59"/>
     </row>
     <row r="464" customHeight="1" spans="1:1">
-      <c r="A464" s="58"/>
+      <c r="A464" s="59"/>
     </row>
     <row r="465" customHeight="1" spans="1:1">
-      <c r="A465" s="58"/>
+      <c r="A465" s="59"/>
     </row>
     <row r="466" customHeight="1" spans="1:1">
-      <c r="A466" s="58"/>
+      <c r="A466" s="59"/>
     </row>
     <row r="467" customHeight="1" spans="1:1">
-      <c r="A467" s="58"/>
+      <c r="A467" s="59"/>
     </row>
     <row r="468" customHeight="1" spans="1:1">
-      <c r="A468" s="58"/>
+      <c r="A468" s="59"/>
     </row>
     <row r="469" customHeight="1" spans="1:1">
-      <c r="A469" s="58"/>
+      <c r="A469" s="59"/>
     </row>
     <row r="470" customHeight="1" spans="1:1">
-      <c r="A470" s="58"/>
+      <c r="A470" s="59"/>
     </row>
     <row r="471" customHeight="1" spans="1:1">
-      <c r="A471" s="58"/>
+      <c r="A471" s="59"/>
     </row>
     <row r="472" customHeight="1" spans="1:1">
-      <c r="A472" s="58"/>
+      <c r="A472" s="59"/>
     </row>
     <row r="473" customHeight="1" spans="1:1">
-      <c r="A473" s="58"/>
+      <c r="A473" s="59"/>
     </row>
     <row r="474" customHeight="1" spans="1:1">
-      <c r="A474" s="58"/>
+      <c r="A474" s="59"/>
     </row>
     <row r="475" customHeight="1" spans="1:1">
-      <c r="A475" s="58"/>
+      <c r="A475" s="59"/>
     </row>
     <row r="476" customHeight="1" spans="1:1">
-      <c r="A476" s="58"/>
+      <c r="A476" s="59"/>
     </row>
     <row r="477" customHeight="1" spans="1:1">
-      <c r="A477" s="58"/>
+      <c r="A477" s="59"/>
     </row>
     <row r="478" customHeight="1" spans="1:1">
-      <c r="A478" s="58"/>
+      <c r="A478" s="59"/>
     </row>
     <row r="479" customHeight="1" spans="1:1">
-      <c r="A479" s="58"/>
+      <c r="A479" s="59"/>
     </row>
     <row r="480" customHeight="1" spans="1:1">
-      <c r="A480" s="58"/>
+      <c r="A480" s="59"/>
     </row>
     <row r="481" customHeight="1" spans="1:1">
-      <c r="A481" s="58"/>
+      <c r="A481" s="59"/>
     </row>
     <row r="482" customHeight="1" spans="1:1">
-      <c r="A482" s="58"/>
+      <c r="A482" s="59"/>
     </row>
     <row r="483" customHeight="1" spans="1:1">
-      <c r="A483" s="58"/>
+      <c r="A483" s="59"/>
     </row>
     <row r="484" customHeight="1" spans="1:1">
-      <c r="A484" s="58"/>
+      <c r="A484" s="59"/>
     </row>
     <row r="485" customHeight="1" spans="1:1">
-      <c r="A485" s="58"/>
+      <c r="A485" s="59"/>
     </row>
     <row r="486" customHeight="1" spans="1:1">
-      <c r="A486" s="58"/>
+      <c r="A486" s="59"/>
     </row>
     <row r="487" customHeight="1" spans="1:1">
-      <c r="A487" s="58"/>
+      <c r="A487" s="59"/>
     </row>
     <row r="488" customHeight="1" spans="1:1">
-      <c r="A488" s="58"/>
+      <c r="A488" s="59"/>
     </row>
     <row r="489" customHeight="1" spans="1:1">
-      <c r="A489" s="58"/>
+      <c r="A489" s="59"/>
     </row>
     <row r="490" customHeight="1" spans="1:1">
-      <c r="A490" s="58"/>
+      <c r="A490" s="59"/>
     </row>
     <row r="491" customHeight="1" spans="1:1">
-      <c r="A491" s="58"/>
+      <c r="A491" s="59"/>
     </row>
     <row r="492" customHeight="1" spans="1:1">
-      <c r="A492" s="58"/>
+      <c r="A492" s="59"/>
     </row>
     <row r="493" customHeight="1" spans="1:1">
-      <c r="A493" s="58"/>
+      <c r="A493" s="59"/>
     </row>
     <row r="494" customHeight="1" spans="1:1">
-      <c r="A494" s="58"/>
+      <c r="A494" s="59"/>
     </row>
     <row r="495" customHeight="1" spans="1:1">
-      <c r="A495" s="58"/>
+      <c r="A495" s="59"/>
     </row>
     <row r="496" customHeight="1" spans="1:1">
-      <c r="A496" s="58"/>
+      <c r="A496" s="59"/>
     </row>
     <row r="497" customHeight="1" spans="1:1">
-      <c r="A497" s="58"/>
+      <c r="A497" s="59"/>
     </row>
     <row r="498" customHeight="1" spans="1:1">
-      <c r="A498" s="58"/>
+      <c r="A498" s="59"/>
     </row>
     <row r="499" customHeight="1" spans="1:1">
-      <c r="A499" s="58"/>
+      <c r="A499" s="59"/>
     </row>
     <row r="500" customHeight="1" spans="1:1">
-      <c r="A500" s="58"/>
+      <c r="A500" s="59"/>
     </row>
     <row r="501" customHeight="1" spans="1:1">
-      <c r="A501" s="58"/>
+      <c r="A501" s="59"/>
     </row>
     <row r="502" customHeight="1" spans="1:1">
-      <c r="A502" s="58"/>
+      <c r="A502" s="59"/>
     </row>
     <row r="503" customHeight="1" spans="1:1">
-      <c r="A503" s="58"/>
+      <c r="A503" s="59"/>
     </row>
     <row r="504" customHeight="1" spans="1:1">
-      <c r="A504" s="58"/>
+      <c r="A504" s="59"/>
     </row>
     <row r="505" customHeight="1" spans="1:1">
-      <c r="A505" s="58"/>
+      <c r="A505" s="59"/>
     </row>
     <row r="506" customHeight="1" spans="1:1">
-      <c r="A506" s="58"/>
+      <c r="A506" s="59"/>
     </row>
     <row r="507" customHeight="1" spans="1:1">
-      <c r="A507" s="58"/>
+      <c r="A507" s="59"/>
     </row>
     <row r="508" customHeight="1" spans="1:1">
-      <c r="A508" s="58"/>
+      <c r="A508" s="59"/>
     </row>
     <row r="509" customHeight="1" spans="1:1">
-      <c r="A509" s="58"/>
+      <c r="A509" s="59"/>
     </row>
     <row r="510" customHeight="1" spans="1:1">
-      <c r="A510" s="58"/>
+      <c r="A510" s="59"/>
     </row>
     <row r="511" customHeight="1" spans="1:1">
-      <c r="A511" s="58"/>
+      <c r="A511" s="59"/>
     </row>
     <row r="512" customHeight="1" spans="1:1">
-      <c r="A512" s="58"/>
+      <c r="A512" s="59"/>
     </row>
     <row r="513" customHeight="1" spans="1:1">
-      <c r="A513" s="58"/>
+      <c r="A513" s="59"/>
     </row>
     <row r="514" customHeight="1" spans="1:1">
-      <c r="A514" s="58"/>
+      <c r="A514" s="59"/>
     </row>
     <row r="515" customHeight="1" spans="1:1">
-      <c r="A515" s="58"/>
+      <c r="A515" s="59"/>
     </row>
     <row r="516" customHeight="1" spans="1:1">
-      <c r="A516" s="58"/>
+      <c r="A516" s="59"/>
     </row>
     <row r="517" customHeight="1" spans="1:1">
-      <c r="A517" s="58"/>
+      <c r="A517" s="59"/>
     </row>
     <row r="518" customHeight="1" spans="1:1">
-      <c r="A518" s="58"/>
+      <c r="A518" s="59"/>
     </row>
     <row r="519" customHeight="1" spans="1:1">
-      <c r="A519" s="58"/>
+      <c r="A519" s="59"/>
     </row>
     <row r="520" customHeight="1" spans="1:1">
-      <c r="A520" s="58"/>
+      <c r="A520" s="59"/>
     </row>
     <row r="521" customHeight="1" spans="1:1">
-      <c r="A521" s="58"/>
+      <c r="A521" s="59"/>
     </row>
     <row r="522" customHeight="1" spans="1:1">
-      <c r="A522" s="58"/>
+      <c r="A522" s="59"/>
     </row>
     <row r="523" customHeight="1" spans="1:1">
-      <c r="A523" s="58"/>
+      <c r="A523" s="59"/>
     </row>
     <row r="524" customHeight="1" spans="1:1">
-      <c r="A524" s="58"/>
+      <c r="A524" s="59"/>
     </row>
     <row r="525" customHeight="1" spans="1:1">
-      <c r="A525" s="58"/>
+      <c r="A525" s="59"/>
     </row>
     <row r="526" customHeight="1" spans="1:1">
-      <c r="A526" s="58"/>
+      <c r="A526" s="59"/>
     </row>
     <row r="527" customHeight="1" spans="1:1">
-      <c r="A527" s="58"/>
+      <c r="A527" s="59"/>
     </row>
     <row r="528" customHeight="1" spans="1:1">
-      <c r="A528" s="58"/>
+      <c r="A528" s="59"/>
     </row>
     <row r="529" customHeight="1" spans="1:1">
-      <c r="A529" s="58"/>
+      <c r="A529" s="59"/>
     </row>
     <row r="530" customHeight="1" spans="1:1">
-      <c r="A530" s="58"/>
+      <c r="A530" s="59"/>
     </row>
     <row r="531" customHeight="1" spans="1:1">
-      <c r="A531" s="58"/>
+      <c r="A531" s="59"/>
     </row>
     <row r="532" customHeight="1" spans="1:1">
-      <c r="A532" s="58"/>
+      <c r="A532" s="59"/>
     </row>
     <row r="533" customHeight="1" spans="1:1">
-      <c r="A533" s="58"/>
+      <c r="A533" s="59"/>
     </row>
     <row r="534" customHeight="1" spans="1:1">
-      <c r="A534" s="58"/>
+      <c r="A534" s="59"/>
     </row>
     <row r="535" customHeight="1" spans="1:1">
-      <c r="A535" s="58"/>
+      <c r="A535" s="59"/>
     </row>
     <row r="536" customHeight="1" spans="1:1">
-      <c r="A536" s="58"/>
+      <c r="A536" s="59"/>
     </row>
     <row r="537" customHeight="1" spans="1:1">
-      <c r="A537" s="58"/>
+      <c r="A537" s="59"/>
     </row>
     <row r="538" customHeight="1" spans="1:1">
-      <c r="A538" s="58"/>
+      <c r="A538" s="59"/>
     </row>
     <row r="539" customHeight="1" spans="1:1">
-      <c r="A539" s="58"/>
+      <c r="A539" s="59"/>
     </row>
     <row r="540" customHeight="1" spans="1:1">
-      <c r="A540" s="58"/>
+      <c r="A540" s="59"/>
     </row>
     <row r="541" customHeight="1" spans="1:1">
-      <c r="A541" s="58"/>
+      <c r="A541" s="59"/>
     </row>
     <row r="542" customHeight="1" spans="1:1">
-      <c r="A542" s="58"/>
+      <c r="A542" s="59"/>
     </row>
     <row r="543" customHeight="1" spans="1:1">
-      <c r="A543" s="58"/>
+      <c r="A543" s="59"/>
     </row>
     <row r="544" customHeight="1" spans="1:1">
-      <c r="A544" s="58"/>
+      <c r="A544" s="59"/>
     </row>
     <row r="545" customHeight="1" spans="1:1">
-      <c r="A545" s="58"/>
+      <c r="A545" s="59"/>
     </row>
     <row r="546" customHeight="1" spans="1:1">
-      <c r="A546" s="58"/>
+      <c r="A546" s="59"/>
     </row>
     <row r="547" customHeight="1" spans="1:1">
-      <c r="A547" s="58"/>
+      <c r="A547" s="59"/>
     </row>
     <row r="548" customHeight="1" spans="1:1">
-      <c r="A548" s="58"/>
+      <c r="A548" s="59"/>
     </row>
     <row r="549" customHeight="1" spans="1:1">
-      <c r="A549" s="58"/>
+      <c r="A549" s="59"/>
     </row>
     <row r="550" customHeight="1" spans="1:1">
-      <c r="A550" s="58"/>
+      <c r="A550" s="59"/>
     </row>
     <row r="551" customHeight="1" spans="1:1">
-      <c r="A551" s="58"/>
+      <c r="A551" s="59"/>
     </row>
     <row r="552" customHeight="1" spans="1:1">
-      <c r="A552" s="58"/>
+      <c r="A552" s="59"/>
     </row>
     <row r="553" customHeight="1" spans="1:1">
-      <c r="A553" s="58"/>
+      <c r="A553" s="59"/>
     </row>
     <row r="554" customHeight="1" spans="1:1">
-      <c r="A554" s="58"/>
+      <c r="A554" s="59"/>
     </row>
     <row r="555" customHeight="1" spans="1:1">
-      <c r="A555" s="58"/>
+      <c r="A555" s="59"/>
     </row>
     <row r="556" customHeight="1" spans="1:1">
-      <c r="A556" s="58"/>
+      <c r="A556" s="59"/>
     </row>
     <row r="557" customHeight="1" spans="1:1">
-      <c r="A557" s="58"/>
+      <c r="A557" s="59"/>
     </row>
     <row r="558" customHeight="1" spans="1:1">
-      <c r="A558" s="58"/>
+      <c r="A558" s="59"/>
     </row>
     <row r="559" customHeight="1" spans="1:1">
-      <c r="A559" s="58"/>
+      <c r="A559" s="59"/>
     </row>
     <row r="560" customHeight="1" spans="1:1">
-      <c r="A560" s="58"/>
+      <c r="A560" s="59"/>
     </row>
     <row r="561" customHeight="1" spans="1:1">
-      <c r="A561" s="58"/>
+      <c r="A561" s="59"/>
     </row>
     <row r="562" customHeight="1" spans="1:1">
-      <c r="A562" s="58"/>
+      <c r="A562" s="59"/>
     </row>
     <row r="563" customHeight="1" spans="1:1">
-      <c r="A563" s="58"/>
+      <c r="A563" s="59"/>
     </row>
     <row r="564" customHeight="1" spans="1:1">
-      <c r="A564" s="58"/>
+      <c r="A564" s="59"/>
     </row>
     <row r="565" customHeight="1" spans="1:1">
-      <c r="A565" s="58"/>
+      <c r="A565" s="59"/>
     </row>
     <row r="566" customHeight="1" spans="1:1">
-      <c r="A566" s="58"/>
+      <c r="A566" s="59"/>
     </row>
     <row r="567" customHeight="1" spans="1:1">
-      <c r="A567" s="58"/>
+      <c r="A567" s="59"/>
     </row>
     <row r="568" customHeight="1" spans="1:1">
-      <c r="A568" s="58"/>
+      <c r="A568" s="59"/>
     </row>
     <row r="569" customHeight="1" spans="1:1">
-      <c r="A569" s="58"/>
+      <c r="A569" s="59"/>
     </row>
     <row r="570" customHeight="1" spans="1:1">
-      <c r="A570" s="58"/>
+      <c r="A570" s="59"/>
     </row>
     <row r="571" customHeight="1" spans="1:1">
-      <c r="A571" s="58"/>
+      <c r="A571" s="59"/>
     </row>
     <row r="572" customHeight="1" spans="1:1">
-      <c r="A572" s="58"/>
+      <c r="A572" s="59"/>
     </row>
     <row r="573" customHeight="1" spans="1:1">
-      <c r="A573" s="58"/>
+      <c r="A573" s="59"/>
     </row>
     <row r="574" customHeight="1" spans="1:1">
-      <c r="A574" s="58"/>
+      <c r="A574" s="59"/>
     </row>
     <row r="575" customHeight="1" spans="1:1">
-      <c r="A575" s="58"/>
+      <c r="A575" s="59"/>
     </row>
     <row r="576" customHeight="1" spans="1:1">
-      <c r="A576" s="58"/>
+      <c r="A576" s="59"/>
     </row>
     <row r="577" customHeight="1" spans="1:1">
-      <c r="A577" s="58"/>
+      <c r="A577" s="59"/>
     </row>
     <row r="578" customHeight="1" spans="1:1">
-      <c r="A578" s="58"/>
+      <c r="A578" s="59"/>
     </row>
     <row r="579" customHeight="1" spans="1:1">
-      <c r="A579" s="58"/>
+      <c r="A579" s="59"/>
     </row>
     <row r="580" customHeight="1" spans="1:1">
-      <c r="A580" s="58"/>
+      <c r="A580" s="59"/>
     </row>
     <row r="581" customHeight="1" spans="1:1">
-      <c r="A581" s="58"/>
+      <c r="A581" s="59"/>
     </row>
     <row r="582" customHeight="1" spans="1:1">
-      <c r="A582" s="58"/>
+      <c r="A582" s="59"/>
     </row>
     <row r="583" customHeight="1" spans="1:1">
-      <c r="A583" s="58"/>
+      <c r="A583" s="59"/>
     </row>
     <row r="584" customHeight="1" spans="1:1">
-      <c r="A584" s="58"/>
+      <c r="A584" s="59"/>
     </row>
     <row r="585" customHeight="1" spans="1:1">
-      <c r="A585" s="58"/>
+      <c r="A585" s="59"/>
     </row>
     <row r="586" customHeight="1" spans="1:1">
-      <c r="A586" s="58"/>
+      <c r="A586" s="59"/>
     </row>
     <row r="587" customHeight="1" spans="1:1">
-      <c r="A587" s="58"/>
+      <c r="A587" s="59"/>
     </row>
     <row r="588" customHeight="1" spans="1:1">
-      <c r="A588" s="58"/>
+      <c r="A588" s="59"/>
     </row>
     <row r="589" customHeight="1" spans="1:1">
-      <c r="A589" s="58"/>
+      <c r="A589" s="59"/>
     </row>
     <row r="590" customHeight="1" spans="1:1">
-      <c r="A590" s="58"/>
+      <c r="A590" s="59"/>
     </row>
     <row r="591" customHeight="1" spans="1:1">
-      <c r="A591" s="58"/>
+      <c r="A591" s="59"/>
     </row>
     <row r="592" customHeight="1" spans="1:1">
-      <c r="A592" s="58"/>
+      <c r="A592" s="59"/>
     </row>
     <row r="593" customHeight="1" spans="1:1">
-      <c r="A593" s="58"/>
+      <c r="A593" s="59"/>
     </row>
     <row r="594" customHeight="1" spans="1:1">
-      <c r="A594" s="58"/>
+      <c r="A594" s="59"/>
     </row>
     <row r="595" customHeight="1" spans="1:1">
-      <c r="A595" s="58"/>
+      <c r="A595" s="59"/>
     </row>
     <row r="596" customHeight="1" spans="1:1">
-      <c r="A596" s="58"/>
+      <c r="A596" s="59"/>
     </row>
     <row r="597" customHeight="1" spans="1:1">
-      <c r="A597" s="58"/>
+      <c r="A597" s="59"/>
     </row>
     <row r="598" customHeight="1" spans="1:1">
-      <c r="A598" s="58"/>
+      <c r="A598" s="59"/>
     </row>
     <row r="599" customHeight="1" spans="1:1">
-      <c r="A599" s="58"/>
+      <c r="A599" s="59"/>
     </row>
     <row r="600" customHeight="1" spans="1:1">
-      <c r="A600" s="58"/>
+      <c r="A600" s="59"/>
     </row>
     <row r="601" customHeight="1" spans="1:1">
-      <c r="A601" s="58"/>
+      <c r="A601" s="59"/>
     </row>
     <row r="602" customHeight="1" spans="1:1">
-      <c r="A602" s="58"/>
+      <c r="A602" s="59"/>
     </row>
     <row r="603" customHeight="1" spans="1:1">
-      <c r="A603" s="58"/>
+      <c r="A603" s="59"/>
     </row>
     <row r="604" customHeight="1" spans="1:1">
-      <c r="A604" s="58"/>
+      <c r="A604" s="59"/>
     </row>
     <row r="605" customHeight="1" spans="1:1">
-      <c r="A605" s="58"/>
+      <c r="A605" s="59"/>
     </row>
     <row r="606" customHeight="1" spans="1:1">
-      <c r="A606" s="58"/>
+      <c r="A606" s="59"/>
     </row>
     <row r="607" customHeight="1" spans="1:1">
-      <c r="A607" s="58"/>
+      <c r="A607" s="59"/>
     </row>
     <row r="608" customHeight="1" spans="1:1">
-      <c r="A608" s="58"/>
+      <c r="A608" s="59"/>
     </row>
     <row r="609" customHeight="1" spans="1:1">
-      <c r="A609" s="58"/>
+      <c r="A609" s="59"/>
     </row>
     <row r="610" customHeight="1" spans="1:1">
-      <c r="A610" s="58"/>
+      <c r="A610" s="59"/>
     </row>
     <row r="611" customHeight="1" spans="1:1">
-      <c r="A611" s="58"/>
+      <c r="A611" s="59"/>
     </row>
     <row r="612" customHeight="1" spans="1:1">
-      <c r="A612" s="58"/>
+      <c r="A612" s="59"/>
     </row>
     <row r="613" customHeight="1" spans="1:1">
-      <c r="A613" s="58"/>
+      <c r="A613" s="59"/>
     </row>
     <row r="614" customHeight="1" spans="1:1">
-      <c r="A614" s="58"/>
+      <c r="A614" s="59"/>
     </row>
     <row r="615" customHeight="1" spans="1:1">
-      <c r="A615" s="58"/>
+      <c r="A615" s="59"/>
     </row>
     <row r="616" customHeight="1" spans="1:1">
-      <c r="A616" s="58"/>
+      <c r="A616" s="59"/>
     </row>
     <row r="617" customHeight="1" spans="1:1">
-      <c r="A617" s="58"/>
+      <c r="A617" s="59"/>
     </row>
     <row r="618" customHeight="1" spans="1:1">
-      <c r="A618" s="58"/>
+      <c r="A618" s="59"/>
     </row>
     <row r="619" customHeight="1" spans="1:1">
-      <c r="A619" s="58"/>
+      <c r="A619" s="59"/>
     </row>
     <row r="620" customHeight="1" spans="1:1">
-      <c r="A620" s="58"/>
+      <c r="A620" s="59"/>
     </row>
     <row r="621" customHeight="1" spans="1:1">
-      <c r="A621" s="58"/>
+      <c r="A621" s="59"/>
     </row>
     <row r="622" customHeight="1" spans="1:1">
-      <c r="A622" s="58"/>
+      <c r="A622" s="59"/>
     </row>
     <row r="623" customHeight="1" spans="1:1">
-      <c r="A623" s="58"/>
+      <c r="A623" s="59"/>
     </row>
     <row r="624" customHeight="1" spans="1:1">
-      <c r="A624" s="58"/>
+      <c r="A624" s="59"/>
     </row>
     <row r="625" customHeight="1" spans="1:1">
-      <c r="A625" s="58"/>
+      <c r="A625" s="59"/>
     </row>
     <row r="626" customHeight="1" spans="1:1">
-      <c r="A626" s="58"/>
+      <c r="A626" s="59"/>
     </row>
     <row r="627" customHeight="1" spans="1:1">
-      <c r="A627" s="58"/>
+      <c r="A627" s="59"/>
     </row>
     <row r="628" customHeight="1" spans="1:1">
-      <c r="A628" s="58"/>
+      <c r="A628" s="59"/>
     </row>
     <row r="629" customHeight="1" spans="1:1">
-      <c r="A629" s="58"/>
+      <c r="A629" s="59"/>
     </row>
     <row r="630" customHeight="1" spans="1:1">
-      <c r="A630" s="58"/>
+      <c r="A630" s="59"/>
     </row>
     <row r="631" customHeight="1" spans="1:1">
-      <c r="A631" s="58"/>
+      <c r="A631" s="59"/>
     </row>
     <row r="632" customHeight="1" spans="1:1">
-      <c r="A632" s="58"/>
+      <c r="A632" s="59"/>
     </row>
     <row r="633" customHeight="1" spans="1:1">
-      <c r="A633" s="58"/>
+      <c r="A633" s="59"/>
     </row>
     <row r="634" customHeight="1" spans="1:1">
-      <c r="A634" s="58"/>
+      <c r="A634" s="59"/>
     </row>
     <row r="635" customHeight="1" spans="1:1">
-      <c r="A635" s="58"/>
+      <c r="A635" s="59"/>
     </row>
     <row r="636" customHeight="1" spans="1:1">
-      <c r="A636" s="58"/>
+      <c r="A636" s="59"/>
     </row>
     <row r="637" customHeight="1" spans="1:1">
-      <c r="A637" s="58"/>
+      <c r="A637" s="59"/>
     </row>
     <row r="638" customHeight="1" spans="1:1">
-      <c r="A638" s="58"/>
+      <c r="A638" s="59"/>
     </row>
     <row r="639" customHeight="1" spans="1:1">
-      <c r="A639" s="58"/>
+      <c r="A639" s="59"/>
     </row>
     <row r="640" customHeight="1" spans="1:1">
-      <c r="A640" s="58"/>
+      <c r="A640" s="59"/>
     </row>
     <row r="641" customHeight="1" spans="1:1">
-      <c r="A641" s="58"/>
+      <c r="A641" s="59"/>
     </row>
     <row r="642" customHeight="1" spans="1:1">
-      <c r="A642" s="58"/>
+      <c r="A642" s="59"/>
     </row>
     <row r="643" customHeight="1" spans="1:1">
-      <c r="A643" s="58"/>
+      <c r="A643" s="59"/>
     </row>
     <row r="644" customHeight="1" spans="1:1">
-      <c r="A644" s="58"/>
+      <c r="A644" s="59"/>
     </row>
     <row r="645" customHeight="1" spans="1:1">
-      <c r="A645" s="58"/>
+      <c r="A645" s="59"/>
     </row>
     <row r="646" customHeight="1" spans="1:1">
-      <c r="A646" s="58"/>
+      <c r="A646" s="59"/>
     </row>
     <row r="647" customHeight="1" spans="1:1">
-      <c r="A647" s="58"/>
+      <c r="A647" s="59"/>
     </row>
     <row r="648" customHeight="1" spans="1:1">
-      <c r="A648" s="58"/>
+      <c r="A648" s="59"/>
     </row>
     <row r="649" customHeight="1" spans="1:1">
-      <c r="A649" s="58"/>
+      <c r="A649" s="59"/>
     </row>
     <row r="650" customHeight="1" spans="1:1">
-      <c r="A650" s="58"/>
+      <c r="A650" s="59"/>
     </row>
     <row r="651" customHeight="1" spans="1:1">
-      <c r="A651" s="58"/>
+      <c r="A651" s="59"/>
     </row>
     <row r="652" customHeight="1" spans="1:1">
-      <c r="A652" s="58"/>
+      <c r="A652" s="59"/>
     </row>
     <row r="653" customHeight="1" spans="1:1">
-      <c r="A653" s="58"/>
+      <c r="A653" s="59"/>
     </row>
     <row r="654" customHeight="1" spans="1:1">
-      <c r="A654" s="58"/>
+      <c r="A654" s="59"/>
     </row>
     <row r="655" customHeight="1" spans="1:1">
-      <c r="A655" s="58"/>
+      <c r="A655" s="59"/>
     </row>
     <row r="656" customHeight="1" spans="1:1">
-      <c r="A656" s="58"/>
+      <c r="A656" s="59"/>
     </row>
     <row r="657" customHeight="1" spans="1:1">
-      <c r="A657" s="58"/>
+      <c r="A657" s="59"/>
     </row>
     <row r="658" customHeight="1" spans="1:1">
-      <c r="A658" s="58"/>
+      <c r="A658" s="59"/>
     </row>
     <row r="659" customHeight="1" spans="1:1">
-      <c r="A659" s="58"/>
+      <c r="A659" s="59"/>
     </row>
     <row r="660" customHeight="1" spans="1:1">
-      <c r="A660" s="58"/>
+      <c r="A660" s="59"/>
     </row>
     <row r="661" customHeight="1" spans="1:1">
-      <c r="A661" s="58"/>
+      <c r="A661" s="59"/>
     </row>
     <row r="662" customHeight="1" spans="1:1">
-      <c r="A662" s="58"/>
+      <c r="A662" s="59"/>
     </row>
     <row r="663" customHeight="1" spans="1:1">
-      <c r="A663" s="58"/>
+      <c r="A663" s="59"/>
     </row>
     <row r="664" customHeight="1" spans="1:1">
-      <c r="A664" s="58"/>
+      <c r="A664" s="59"/>
     </row>
     <row r="665" customHeight="1" spans="1:1">
-      <c r="A665" s="58"/>
+      <c r="A665" s="59"/>
     </row>
     <row r="666" customHeight="1" spans="1:1">
-      <c r="A666" s="58"/>
+      <c r="A666" s="59"/>
     </row>
     <row r="667" customHeight="1" spans="1:1">
-      <c r="A667" s="58"/>
+      <c r="A667" s="59"/>
     </row>
     <row r="668" customHeight="1" spans="1:1">
-      <c r="A668" s="58"/>
+      <c r="A668" s="59"/>
     </row>
     <row r="669" customHeight="1" spans="1:1">
-      <c r="A669" s="58"/>
+      <c r="A669" s="59"/>
     </row>
     <row r="670" customHeight="1" spans="1:1">
-      <c r="A670" s="58"/>
+      <c r="A670" s="59"/>
     </row>
     <row r="671" customHeight="1" spans="1:1">
-      <c r="A671" s="58"/>
+      <c r="A671" s="59"/>
     </row>
     <row r="672" customHeight="1" spans="1:1">
-      <c r="A672" s="58"/>
+      <c r="A672" s="59"/>
     </row>
     <row r="673" customHeight="1" spans="1:1">
-      <c r="A673" s="58"/>
+      <c r="A673" s="59"/>
     </row>
     <row r="674" customHeight="1" spans="1:1">
-      <c r="A674" s="58"/>
+      <c r="A674" s="59"/>
     </row>
     <row r="675" customHeight="1" spans="1:1">
-      <c r="A675" s="58"/>
+      <c r="A675" s="59"/>
     </row>
     <row r="676" customHeight="1" spans="1:1">
-      <c r="A676" s="58"/>
+      <c r="A676" s="59"/>
     </row>
     <row r="677" customHeight="1" spans="1:1">
-      <c r="A677" s="58"/>
+      <c r="A677" s="59"/>
     </row>
     <row r="678" customHeight="1" spans="1:1">
-      <c r="A678" s="58"/>
+      <c r="A678" s="59"/>
     </row>
     <row r="679" customHeight="1" spans="1:1">
-      <c r="A679" s="58"/>
+      <c r="A679" s="59"/>
     </row>
     <row r="680" customHeight="1" spans="1:1">
-      <c r="A680" s="58"/>
+      <c r="A680" s="59"/>
     </row>
     <row r="681" customHeight="1" spans="1:1">
-      <c r="A681" s="58"/>
+      <c r="A681" s="59"/>
     </row>
     <row r="682" customHeight="1" spans="1:1">
-      <c r="A682" s="58"/>
+      <c r="A682" s="59"/>
     </row>
     <row r="683" customHeight="1" spans="1:1">
-      <c r="A683" s="58"/>
+      <c r="A683" s="59"/>
     </row>
     <row r="684" customHeight="1" spans="1:1">
-      <c r="A684" s="58"/>
+      <c r="A684" s="59"/>
     </row>
     <row r="685" customHeight="1" spans="1:1">
-      <c r="A685" s="58"/>
+      <c r="A685" s="59"/>
     </row>
     <row r="686" customHeight="1" spans="1:1">
-      <c r="A686" s="58"/>
+      <c r="A686" s="59"/>
     </row>
     <row r="687" customHeight="1" spans="1:1">
-      <c r="A687" s="58"/>
+      <c r="A687" s="59"/>
     </row>
     <row r="688" customHeight="1" spans="1:1">
-      <c r="A688" s="58"/>
+      <c r="A688" s="59"/>
     </row>
     <row r="689" customHeight="1" spans="1:1">
-      <c r="A689" s="58"/>
+      <c r="A689" s="59"/>
     </row>
     <row r="690" customHeight="1" spans="1:1">
-      <c r="A690" s="58"/>
+      <c r="A690" s="59"/>
     </row>
     <row r="691" customHeight="1" spans="1:1">
-      <c r="A691" s="58"/>
+      <c r="A691" s="59"/>
     </row>
     <row r="692" customHeight="1" spans="1:1">
-      <c r="A692" s="58"/>
+      <c r="A692" s="59"/>
     </row>
     <row r="693" customHeight="1" spans="1:1">
-      <c r="A693" s="58"/>
+      <c r="A693" s="59"/>
     </row>
     <row r="694" customHeight="1" spans="1:1">
-      <c r="A694" s="58"/>
+      <c r="A694" s="59"/>
     </row>
     <row r="695" customHeight="1" spans="1:1">
-      <c r="A695" s="58"/>
+      <c r="A695" s="59"/>
     </row>
     <row r="696" customHeight="1" spans="1:1">
-      <c r="A696" s="58"/>
+      <c r="A696" s="59"/>
     </row>
     <row r="697" customHeight="1" spans="1:1">
-      <c r="A697" s="58"/>
+      <c r="A697" s="59"/>
     </row>
     <row r="698" customHeight="1" spans="1:1">
-      <c r="A698" s="58"/>
+      <c r="A698" s="59"/>
     </row>
     <row r="699" customHeight="1" spans="1:1">
-      <c r="A699" s="58"/>
+      <c r="A699" s="59"/>
     </row>
     <row r="700" customHeight="1" spans="1:1">
-      <c r="A700" s="58"/>
+      <c r="A700" s="59"/>
     </row>
     <row r="701" customHeight="1" spans="1:1">
-      <c r="A701" s="58"/>
+      <c r="A701" s="59"/>
     </row>
     <row r="702" customHeight="1" spans="1:1">
-      <c r="A702" s="58"/>
+      <c r="A702" s="59"/>
     </row>
     <row r="703" customHeight="1" spans="1:1">
-      <c r="A703" s="58"/>
+      <c r="A703" s="59"/>
     </row>
     <row r="704" customHeight="1" spans="1:1">
-      <c r="A704" s="58"/>
+      <c r="A704" s="59"/>
     </row>
     <row r="705" customHeight="1" spans="1:1">
-      <c r="A705" s="58"/>
+      <c r="A705" s="59"/>
     </row>
     <row r="706" customHeight="1" spans="1:1">
-      <c r="A706" s="58"/>
+      <c r="A706" s="59"/>
     </row>
     <row r="707" customHeight="1" spans="1:1">
-      <c r="A707" s="58"/>
+      <c r="A707" s="59"/>
     </row>
     <row r="708" customHeight="1" spans="1:1">
-      <c r="A708" s="58"/>
+      <c r="A708" s="59"/>
     </row>
     <row r="709" customHeight="1" spans="1:1">
-      <c r="A709" s="58"/>
+      <c r="A709" s="59"/>
     </row>
     <row r="710" customHeight="1" spans="1:1">
-      <c r="A710" s="58"/>
+      <c r="A710" s="59"/>
     </row>
     <row r="711" customHeight="1" spans="1:1">
-      <c r="A711" s="58"/>
+      <c r="A711" s="59"/>
     </row>
     <row r="712" customHeight="1" spans="1:1">
-      <c r="A712" s="58"/>
+      <c r="A712" s="59"/>
     </row>
     <row r="713" customHeight="1" spans="1:1">
-      <c r="A713" s="58"/>
+      <c r="A713" s="59"/>
     </row>
     <row r="714" customHeight="1" spans="1:1">
-      <c r="A714" s="58"/>
+      <c r="A714" s="59"/>
     </row>
     <row r="715" customHeight="1" spans="1:1">
-      <c r="A715" s="58"/>
+      <c r="A715" s="59"/>
     </row>
     <row r="716" customHeight="1" spans="1:1">
-      <c r="A716" s="58"/>
+      <c r="A716" s="59"/>
     </row>
     <row r="717" customHeight="1" spans="1:1">
-      <c r="A717" s="58"/>
+      <c r="A717" s="59"/>
     </row>
     <row r="718" customHeight="1" spans="1:1">
-      <c r="A718" s="58"/>
+      <c r="A718" s="59"/>
     </row>
     <row r="719" customHeight="1" spans="1:1">
-      <c r="A719" s="58"/>
+      <c r="A719" s="59"/>
     </row>
     <row r="720" customHeight="1" spans="1:1">
-      <c r="A720" s="58"/>
+      <c r="A720" s="59"/>
     </row>
     <row r="721" customHeight="1" spans="1:1">
-      <c r="A721" s="58"/>
+      <c r="A721" s="59"/>
     </row>
     <row r="722" customHeight="1" spans="1:1">
-      <c r="A722" s="58"/>
+      <c r="A722" s="59"/>
     </row>
     <row r="723" customHeight="1" spans="1:1">
-      <c r="A723" s="58"/>
+      <c r="A723" s="59"/>
     </row>
     <row r="724" customHeight="1" spans="1:1">
-      <c r="A724" s="58"/>
+      <c r="A724" s="59"/>
     </row>
     <row r="725" customHeight="1" spans="1:1">
-      <c r="A725" s="58"/>
+      <c r="A725" s="59"/>
     </row>
     <row r="726" customHeight="1" spans="1:1">
-      <c r="A726" s="58"/>
+      <c r="A726" s="59"/>
     </row>
     <row r="727" customHeight="1" spans="1:1">
-      <c r="A727" s="58"/>
+      <c r="A727" s="59"/>
     </row>
     <row r="728" customHeight="1" spans="1:1">
-      <c r="A728" s="58"/>
+      <c r="A728" s="59"/>
     </row>
     <row r="729" customHeight="1" spans="1:1">
-      <c r="A729" s="58"/>
+      <c r="A729" s="59"/>
     </row>
     <row r="730" customHeight="1" spans="1:1">
-      <c r="A730" s="58"/>
+      <c r="A730" s="59"/>
     </row>
     <row r="731" customHeight="1" spans="1:1">
-      <c r="A731" s="58"/>
+      <c r="A731" s="59"/>
     </row>
     <row r="732" customHeight="1" spans="1:1">
-      <c r="A732" s="58"/>
+      <c r="A732" s="59"/>
     </row>
     <row r="733" customHeight="1" spans="1:1">
-      <c r="A733" s="58"/>
+      <c r="A733" s="59"/>
     </row>
     <row r="734" customHeight="1" spans="1:1">
-      <c r="A734" s="58"/>
+      <c r="A734" s="59"/>
     </row>
     <row r="735" customHeight="1" spans="1:1">
-      <c r="A735" s="58"/>
+      <c r="A735" s="59"/>
     </row>
     <row r="736" customHeight="1" spans="1:1">
-      <c r="A736" s="58"/>
+      <c r="A736" s="59"/>
     </row>
     <row r="737" customHeight="1" spans="1:1">
-      <c r="A737" s="58"/>
+      <c r="A737" s="59"/>
     </row>
     <row r="738" customHeight="1" spans="1:1">
-      <c r="A738" s="58"/>
+      <c r="A738" s="59"/>
     </row>
     <row r="739" customHeight="1" spans="1:1">
-      <c r="A739" s="58"/>
+      <c r="A739" s="59"/>
     </row>
     <row r="740" customHeight="1" spans="1:1">
-      <c r="A740" s="58"/>
+      <c r="A740" s="59"/>
     </row>
     <row r="741" customHeight="1" spans="1:1">
-      <c r="A741" s="58"/>
+      <c r="A741" s="59"/>
     </row>
     <row r="742" customHeight="1" spans="1:1">
-      <c r="A742" s="58"/>
+      <c r="A742" s="59"/>
     </row>
     <row r="743" customHeight="1" spans="1:1">
-      <c r="A743" s="58"/>
+      <c r="A743" s="59"/>
     </row>
     <row r="744" customHeight="1" spans="1:1">
-      <c r="A744" s="58"/>
+      <c r="A744" s="59"/>
     </row>
     <row r="745" customHeight="1" spans="1:1">
-      <c r="A745" s="58"/>
+      <c r="A745" s="59"/>
     </row>
     <row r="746" customHeight="1" spans="1:1">
-      <c r="A746" s="58"/>
+      <c r="A746" s="59"/>
     </row>
     <row r="747" customHeight="1" spans="1:1">
-      <c r="A747" s="58"/>
+      <c r="A747" s="59"/>
     </row>
     <row r="748" customHeight="1" spans="1:1">
-      <c r="A748" s="58"/>
+      <c r="A748" s="59"/>
     </row>
     <row r="749" customHeight="1" spans="1:1">
-      <c r="A749" s="58"/>
+      <c r="A749" s="59"/>
     </row>
     <row r="750" customHeight="1" spans="1:1">
-      <c r="A750" s="58"/>
+      <c r="A750" s="59"/>
     </row>
     <row r="751" customHeight="1" spans="1:1">
-      <c r="A751" s="58"/>
+      <c r="A751" s="59"/>
     </row>
     <row r="752" customHeight="1" spans="1:1">
-      <c r="A752" s="58"/>
+      <c r="A752" s="59"/>
     </row>
     <row r="753" customHeight="1" spans="1:1">
-      <c r="A753" s="58"/>
+      <c r="A753" s="59"/>
     </row>
     <row r="754" customHeight="1" spans="1:1">
-      <c r="A754" s="58"/>
+      <c r="A754" s="59"/>
     </row>
     <row r="755" customHeight="1" spans="1:1">
-      <c r="A755" s="58"/>
+      <c r="A755" s="59"/>
     </row>
     <row r="756" customHeight="1" spans="1:1">
-      <c r="A756" s="58"/>
+      <c r="A756" s="59"/>
     </row>
     <row r="757" customHeight="1" spans="1:1">
-      <c r="A757" s="58"/>
+      <c r="A757" s="59"/>
     </row>
     <row r="758" customHeight="1" spans="1:1">
-      <c r="A758" s="58"/>
+      <c r="A758" s="59"/>
     </row>
     <row r="759" customHeight="1" spans="1:1">
-      <c r="A759" s="58"/>
+      <c r="A759" s="59"/>
     </row>
     <row r="760" customHeight="1" spans="1:1">
-      <c r="A760" s="58"/>
+      <c r="A760" s="59"/>
     </row>
     <row r="761" customHeight="1" spans="1:1">
-      <c r="A761" s="58"/>
+      <c r="A761" s="59"/>
     </row>
     <row r="762" customHeight="1" spans="1:1">
-      <c r="A762" s="58"/>
+      <c r="A762" s="59"/>
     </row>
     <row r="763" customHeight="1" spans="1:1">
-      <c r="A763" s="58"/>
+      <c r="A763" s="59"/>
     </row>
     <row r="764" customHeight="1" spans="1:1">
-      <c r="A764" s="58"/>
+      <c r="A764" s="59"/>
     </row>
     <row r="765" customHeight="1" spans="1:1">
-      <c r="A765" s="58"/>
+      <c r="A765" s="59"/>
     </row>
     <row r="766" customHeight="1" spans="1:1">
-      <c r="A766" s="58"/>
+      <c r="A766" s="59"/>
     </row>
     <row r="767" customHeight="1" spans="1:1">
-      <c r="A767" s="58"/>
+      <c r="A767" s="59"/>
     </row>
     <row r="768" customHeight="1" spans="1:1">
-      <c r="A768" s="58"/>
+      <c r="A768" s="59"/>
     </row>
     <row r="769" customHeight="1" spans="1:1">
-      <c r="A769" s="58"/>
+      <c r="A769" s="59"/>
     </row>
     <row r="770" customHeight="1" spans="1:1">
-      <c r="A770" s="58"/>
+      <c r="A770" s="59"/>
     </row>
     <row r="771" customHeight="1" spans="1:1">
-      <c r="A771" s="58"/>
+      <c r="A771" s="59"/>
     </row>
     <row r="772" customHeight="1" spans="1:1">
-      <c r="A772" s="58"/>
+      <c r="A772" s="59"/>
     </row>
     <row r="773" customHeight="1" spans="1:1">
-      <c r="A773" s="58"/>
+      <c r="A773" s="59"/>
     </row>
     <row r="774" customHeight="1" spans="1:1">
-      <c r="A774" s="58"/>
+      <c r="A774" s="59"/>
     </row>
     <row r="775" customHeight="1" spans="1:1">
-      <c r="A775" s="58"/>
+      <c r="A775" s="59"/>
     </row>
     <row r="776" customHeight="1" spans="1:1">
-      <c r="A776" s="58"/>
+      <c r="A776" s="59"/>
     </row>
     <row r="777" customHeight="1" spans="1:1">
-      <c r="A777" s="58"/>
+      <c r="A777" s="59"/>
     </row>
     <row r="778" customHeight="1" spans="1:1">
-      <c r="A778" s="58"/>
+      <c r="A778" s="59"/>
     </row>
     <row r="779" customHeight="1" spans="1:1">
-      <c r="A779" s="58"/>
+      <c r="A779" s="59"/>
     </row>
     <row r="780" customHeight="1" spans="1:1">
-      <c r="A780" s="58"/>
+      <c r="A780" s="59"/>
     </row>
     <row r="781" customHeight="1" spans="1:1">
-      <c r="A781" s="58"/>
+      <c r="A781" s="59"/>
     </row>
     <row r="782" customHeight="1" spans="1:1">
-      <c r="A782" s="58"/>
+      <c r="A782" s="59"/>
     </row>
     <row r="783" customHeight="1" spans="1:1">
-      <c r="A783" s="58"/>
+      <c r="A783" s="59"/>
     </row>
     <row r="784" customHeight="1" spans="1:1">
-      <c r="A784" s="58"/>
+      <c r="A784" s="59"/>
     </row>
     <row r="785" customHeight="1" spans="1:1">
-      <c r="A785" s="58"/>
+      <c r="A785" s="59"/>
     </row>
     <row r="786" customHeight="1" spans="1:1">
-      <c r="A786" s="58"/>
+      <c r="A786" s="59"/>
     </row>
     <row r="787" customHeight="1" spans="1:1">
-      <c r="A787" s="58"/>
+      <c r="A787" s="59"/>
     </row>
     <row r="788" customHeight="1" spans="1:1">
-      <c r="A788" s="58"/>
+      <c r="A788" s="59"/>
     </row>
     <row r="789" customHeight="1" spans="1:1">
-      <c r="A789" s="58"/>
+      <c r="A789" s="59"/>
     </row>
     <row r="790" customHeight="1" spans="1:1">
-      <c r="A790" s="58"/>
+      <c r="A790" s="59"/>
     </row>
     <row r="791" customHeight="1" spans="1:1">
-      <c r="A791" s="58"/>
+      <c r="A791" s="59"/>
     </row>
     <row r="792" customHeight="1" spans="1:1">
-      <c r="A792" s="58"/>
+      <c r="A792" s="59"/>
     </row>
     <row r="793" customHeight="1" spans="1:1">
-      <c r="A793" s="58"/>
+      <c r="A793" s="59"/>
     </row>
     <row r="794" customHeight="1" spans="1:1">
-      <c r="A794" s="58"/>
+      <c r="A794" s="59"/>
     </row>
     <row r="795" customHeight="1" spans="1:1">
-      <c r="A795" s="58"/>
+      <c r="A795" s="59"/>
     </row>
     <row r="796" customHeight="1" spans="1:1">
-      <c r="A796" s="58"/>
+      <c r="A796" s="59"/>
     </row>
     <row r="797" customHeight="1" spans="1:1">
-      <c r="A797" s="58"/>
+      <c r="A797" s="59"/>
     </row>
     <row r="798" customHeight="1" spans="1:1">
-      <c r="A798" s="58"/>
+      <c r="A798" s="59"/>
     </row>
     <row r="799" customHeight="1" spans="1:1">
-      <c r="A799" s="58"/>
+      <c r="A799" s="59"/>
     </row>
     <row r="800" customHeight="1" spans="1:1">
-      <c r="A800" s="58"/>
+      <c r="A800" s="59"/>
     </row>
     <row r="801" customHeight="1" spans="1:1">
-      <c r="A801" s="58"/>
+      <c r="A801" s="59"/>
     </row>
     <row r="802" customHeight="1" spans="1:1">
-      <c r="A802" s="58"/>
+      <c r="A802" s="59"/>
     </row>
     <row r="803" customHeight="1" spans="1:1">
-      <c r="A803" s="58"/>
+      <c r="A803" s="59"/>
     </row>
     <row r="804" customHeight="1" spans="1:1">
-      <c r="A804" s="58"/>
+      <c r="A804" s="59"/>
     </row>
     <row r="805" customHeight="1" spans="1:1">
-      <c r="A805" s="58"/>
+      <c r="A805" s="59"/>
     </row>
     <row r="806" customHeight="1" spans="1:1">
-      <c r="A806" s="58"/>
+      <c r="A806" s="59"/>
     </row>
     <row r="807" customHeight="1" spans="1:1">
-      <c r="A807" s="58"/>
+      <c r="A807" s="59"/>
     </row>
     <row r="808" customHeight="1" spans="1:1">
-      <c r="A808" s="58"/>
+      <c r="A808" s="59"/>
     </row>
     <row r="809" customHeight="1" spans="1:1">
-      <c r="A809" s="58"/>
+      <c r="A809" s="59"/>
     </row>
     <row r="810" customHeight="1" spans="1:1">
-      <c r="A810" s="58"/>
+      <c r="A810" s="59"/>
     </row>
     <row r="811" customHeight="1" spans="1:1">
-      <c r="A811" s="58"/>
+      <c r="A811" s="59"/>
     </row>
     <row r="812" customHeight="1" spans="1:1">
-      <c r="A812" s="58"/>
+      <c r="A812" s="59"/>
     </row>
     <row r="813" customHeight="1" spans="1:1">
-      <c r="A813" s="58"/>
+      <c r="A813" s="59"/>
     </row>
     <row r="814" customHeight="1" spans="1:1">
-      <c r="A814" s="58"/>
+      <c r="A814" s="59"/>
     </row>
     <row r="815" customHeight="1" spans="1:1">
-      <c r="A815" s="58"/>
+      <c r="A815" s="59"/>
     </row>
     <row r="816" customHeight="1" spans="1:1">
-      <c r="A816" s="58"/>
+      <c r="A816" s="59"/>
     </row>
     <row r="817" customHeight="1" spans="1:1">
-      <c r="A817" s="58"/>
+      <c r="A817" s="59"/>
     </row>
     <row r="818" customHeight="1" spans="1:1">
-      <c r="A818" s="58"/>
+      <c r="A818" s="59"/>
     </row>
     <row r="819" customHeight="1" spans="1:1">
-      <c r="A819" s="58"/>
+      <c r="A819" s="59"/>
     </row>
     <row r="820" customHeight="1" spans="1:1">
-      <c r="A820" s="58"/>
+      <c r="A820" s="59"/>
     </row>
     <row r="821" customHeight="1" spans="1:1">
-      <c r="A821" s="58"/>
+      <c r="A821" s="59"/>
     </row>
     <row r="822" customHeight="1" spans="1:1">
-      <c r="A822" s="58"/>
+      <c r="A822" s="59"/>
     </row>
     <row r="823" customHeight="1" spans="1:1">
-      <c r="A823" s="58"/>
+      <c r="A823" s="59"/>
     </row>
     <row r="824" customHeight="1" spans="1:1">
-      <c r="A824" s="58"/>
+      <c r="A824" s="59"/>
     </row>
     <row r="825" customHeight="1" spans="1:1">
-      <c r="A825" s="58"/>
+      <c r="A825" s="59"/>
     </row>
     <row r="826" customHeight="1" spans="1:1">
-      <c r="A826" s="58"/>
+      <c r="A826" s="59"/>
     </row>
     <row r="827" customHeight="1" spans="1:1">
-      <c r="A827" s="58"/>
+      <c r="A827" s="59"/>
     </row>
     <row r="828" customHeight="1" spans="1:1">
-      <c r="A828" s="58"/>
+      <c r="A828" s="59"/>
     </row>
     <row r="829" customHeight="1" spans="1:1">
-      <c r="A829" s="58"/>
+      <c r="A829" s="59"/>
     </row>
     <row r="830" customHeight="1" spans="1:1">
-      <c r="A830" s="58"/>
+      <c r="A830" s="59"/>
     </row>
     <row r="831" customHeight="1" spans="1:1">
-      <c r="A831" s="58"/>
+      <c r="A831" s="59"/>
     </row>
     <row r="832" customHeight="1" spans="1:1">
-      <c r="A832" s="58"/>
+      <c r="A832" s="59"/>
     </row>
     <row r="833" customHeight="1" spans="1:1">
-      <c r="A833" s="58"/>
+      <c r="A833" s="59"/>
     </row>
     <row r="834" customHeight="1" spans="1:1">
-      <c r="A834" s="58"/>
+      <c r="A834" s="59"/>
     </row>
     <row r="835" customHeight="1" spans="1:1">
-      <c r="A835" s="58"/>
+      <c r="A835" s="59"/>
     </row>
     <row r="836" customHeight="1" spans="1:1">
-      <c r="A836" s="58"/>
+      <c r="A836" s="59"/>
     </row>
     <row r="837" customHeight="1" spans="1:1">
-      <c r="A837" s="58"/>
+      <c r="A837" s="59"/>
     </row>
     <row r="838" customHeight="1" spans="1:1">
-      <c r="A838" s="58"/>
+      <c r="A838" s="59"/>
     </row>
     <row r="839" customHeight="1" spans="1:1">
-      <c r="A839" s="58"/>
+      <c r="A839" s="59"/>
     </row>
     <row r="840" customHeight="1" spans="1:1">
-      <c r="A840" s="58"/>
+      <c r="A840" s="59"/>
     </row>
     <row r="841" customHeight="1" spans="1:1">
-      <c r="A841" s="58"/>
+      <c r="A841" s="59"/>
     </row>
     <row r="842" customHeight="1" spans="1:1">
-      <c r="A842" s="58"/>
+      <c r="A842" s="59"/>
     </row>
     <row r="843" customHeight="1" spans="1:1">
-      <c r="A843" s="58"/>
+      <c r="A843" s="59"/>
     </row>
     <row r="844" customHeight="1" spans="1:1">
-      <c r="A844" s="58"/>
+      <c r="A844" s="59"/>
     </row>
     <row r="845" customHeight="1" spans="1:1">
-      <c r="A845" s="58"/>
+      <c r="A845" s="59"/>
     </row>
     <row r="846" customHeight="1" spans="1:1">
-      <c r="A846" s="58"/>
+      <c r="A846" s="59"/>
     </row>
     <row r="847" customHeight="1" spans="1:1">
-      <c r="A847" s="58"/>
+      <c r="A847" s="59"/>
     </row>
     <row r="848" customHeight="1" spans="1:1">
-      <c r="A848" s="58"/>
+      <c r="A848" s="59"/>
     </row>
     <row r="849" customHeight="1" spans="1:1">
-      <c r="A849" s="58"/>
+      <c r="A849" s="59"/>
     </row>
     <row r="850" customHeight="1" spans="1:1">
-      <c r="A850" s="58"/>
+      <c r="A850" s="59"/>
     </row>
     <row r="851" customHeight="1" spans="1:1">
-      <c r="A851" s="58"/>
+      <c r="A851" s="59"/>
     </row>
     <row r="852" customHeight="1" spans="1:1">
-      <c r="A852" s="58"/>
+      <c r="A852" s="59"/>
     </row>
     <row r="853" customHeight="1" spans="1:1">
-      <c r="A853" s="58"/>
+      <c r="A853" s="59"/>
     </row>
     <row r="854" customHeight="1" spans="1:1">
-      <c r="A854" s="58"/>
+      <c r="A854" s="59"/>
     </row>
     <row r="855" customHeight="1" spans="1:1">
-      <c r="A855" s="58"/>
+      <c r="A855" s="59"/>
     </row>
     <row r="856" customHeight="1" spans="1:1">
-      <c r="A856" s="58"/>
+      <c r="A856" s="59"/>
     </row>
     <row r="857" customHeight="1" spans="1:1">
-      <c r="A857" s="58"/>
+      <c r="A857" s="59"/>
     </row>
     <row r="858" customHeight="1" spans="1:1">
-      <c r="A858" s="58"/>
+      <c r="A858" s="59"/>
     </row>
     <row r="859" customHeight="1" spans="1:1">
-      <c r="A859" s="58"/>
+      <c r="A859" s="59"/>
     </row>
     <row r="860" customHeight="1" spans="1:1">
-      <c r="A860" s="58"/>
+      <c r="A860" s="59"/>
     </row>
     <row r="861" customHeight="1" spans="1:1">
-      <c r="A861" s="58"/>
+      <c r="A861" s="59"/>
     </row>
     <row r="862" customHeight="1" spans="1:1">
-      <c r="A862" s="58"/>
+      <c r="A862" s="59"/>
     </row>
     <row r="863" customHeight="1" spans="1:1">
-      <c r="A863" s="58"/>
+      <c r="A863" s="59"/>
     </row>
     <row r="864" customHeight="1" spans="1:1">
-      <c r="A864" s="58"/>
+      <c r="A864" s="59"/>
     </row>
     <row r="865" customHeight="1" spans="1:1">
-      <c r="A865" s="58"/>
+      <c r="A865" s="59"/>
     </row>
     <row r="866" customHeight="1" spans="1:1">
-      <c r="A866" s="58"/>
+      <c r="A866" s="59"/>
     </row>
     <row r="867" customHeight="1" spans="1:1">
-      <c r="A867" s="58"/>
+      <c r="A867" s="59"/>
     </row>
     <row r="868" customHeight="1" spans="1:1">
-      <c r="A868" s="58"/>
+      <c r="A868" s="59"/>
     </row>
     <row r="869" customHeight="1" spans="1:1">
-      <c r="A869" s="58"/>
+      <c r="A869" s="59"/>
     </row>
     <row r="870" customHeight="1" spans="1:1">
-      <c r="A870" s="58"/>
+      <c r="A870" s="59"/>
     </row>
     <row r="871" customHeight="1" spans="1:1">
-      <c r="A871" s="58"/>
+      <c r="A871" s="59"/>
     </row>
     <row r="872" customHeight="1" spans="1:1">
-      <c r="A872" s="58"/>
+      <c r="A872" s="59"/>
     </row>
     <row r="873" customHeight="1" spans="1:1">
-      <c r="A873" s="58"/>
+      <c r="A873" s="59"/>
     </row>
     <row r="874" customHeight="1" spans="1:1">
-      <c r="A874" s="58"/>
+      <c r="A874" s="59"/>
     </row>
     <row r="875" customHeight="1" spans="1:1">
-      <c r="A875" s="58"/>
+      <c r="A875" s="59"/>
     </row>
     <row r="876" customHeight="1" spans="1:1">
-      <c r="A876" s="58"/>
+      <c r="A876" s="59"/>
     </row>
     <row r="877" customHeight="1" spans="1:1">
-      <c r="A877" s="58"/>
+      <c r="A877" s="59"/>
     </row>
     <row r="878" customHeight="1" spans="1:1">
-      <c r="A878" s="58"/>
+      <c r="A878" s="59"/>
     </row>
     <row r="879" customHeight="1" spans="1:1">
-      <c r="A879" s="58"/>
+      <c r="A879" s="59"/>
     </row>
     <row r="880" customHeight="1" spans="1:1">
-      <c r="A880" s="58"/>
+      <c r="A880" s="59"/>
     </row>
     <row r="881" customHeight="1" spans="1:1">
-      <c r="A881" s="58"/>
+      <c r="A881" s="59"/>
     </row>
     <row r="882" customHeight="1" spans="1:1">
-      <c r="A882" s="58"/>
+      <c r="A882" s="59"/>
     </row>
     <row r="883" customHeight="1" spans="1:1">
-      <c r="A883" s="58"/>
+      <c r="A883" s="59"/>
     </row>
     <row r="884" customHeight="1" spans="1:1">
-      <c r="A884" s="58"/>
+      <c r="A884" s="59"/>
     </row>
     <row r="885" customHeight="1" spans="1:1">
-      <c r="A885" s="58"/>
+      <c r="A885" s="59"/>
     </row>
     <row r="886" customHeight="1" spans="1:1">
-      <c r="A886" s="58"/>
+      <c r="A886" s="59"/>
     </row>
     <row r="887" customHeight="1" spans="1:1">
-      <c r="A887" s="58"/>
+      <c r="A887" s="59"/>
     </row>
     <row r="888" customHeight="1" spans="1:1">
-      <c r="A888" s="58"/>
+      <c r="A888" s="59"/>
     </row>
     <row r="889" customHeight="1" spans="1:1">
-      <c r="A889" s="58"/>
+      <c r="A889" s="59"/>
     </row>
     <row r="890" customHeight="1" spans="1:1">
-      <c r="A890" s="58"/>
+      <c r="A890" s="59"/>
     </row>
     <row r="891" customHeight="1" spans="1:1">
-      <c r="A891" s="58"/>
+      <c r="A891" s="59"/>
     </row>
     <row r="892" customHeight="1" spans="1:1">
-      <c r="A892" s="58"/>
+      <c r="A892" s="59"/>
     </row>
     <row r="893" customHeight="1" spans="1:1">
-      <c r="A893" s="58"/>
+      <c r="A893" s="59"/>
     </row>
     <row r="894" customHeight="1" spans="1:1">
-      <c r="A894" s="58"/>
+      <c r="A894" s="59"/>
     </row>
     <row r="895" customHeight="1" spans="1:1">
-      <c r="A895" s="58"/>
+      <c r="A895" s="59"/>
     </row>
     <row r="896" customHeight="1" spans="1:1">
-      <c r="A896" s="58"/>
+      <c r="A896" s="59"/>
     </row>
     <row r="897" customHeight="1" spans="1:1">
-      <c r="A897" s="58"/>
+      <c r="A897" s="59"/>
     </row>
     <row r="898" customHeight="1" spans="1:1">
-      <c r="A898" s="58"/>
+      <c r="A898" s="59"/>
     </row>
     <row r="899" customHeight="1" spans="1:1">
-      <c r="A899" s="58"/>
+      <c r="A899" s="59"/>
     </row>
     <row r="900" customHeight="1" spans="1:1">
-      <c r="A900" s="58"/>
+      <c r="A900" s="59"/>
     </row>
     <row r="901" customHeight="1" spans="1:1">
-      <c r="A901" s="58"/>
+      <c r="A901" s="59"/>
     </row>
     <row r="902" customHeight="1" spans="1:1">
-      <c r="A902" s="58"/>
+      <c r="A902" s="59"/>
     </row>
     <row r="903" customHeight="1" spans="1:1">
-      <c r="A903" s="58"/>
+      <c r="A903" s="59"/>
     </row>
     <row r="904" customHeight="1" spans="1:1">
-      <c r="A904" s="58"/>
+      <c r="A904" s="59"/>
     </row>
     <row r="905" customHeight="1" spans="1:1">
-      <c r="A905" s="58"/>
+      <c r="A905" s="59"/>
     </row>
     <row r="906" customHeight="1" spans="1:1">
-      <c r="A906" s="58"/>
+      <c r="A906" s="59"/>
     </row>
     <row r="907" customHeight="1" spans="1:1">
-      <c r="A907" s="58"/>
+      <c r="A907" s="59"/>
     </row>
     <row r="908" customHeight="1" spans="1:1">
-      <c r="A908" s="58"/>
+      <c r="A908" s="59"/>
     </row>
     <row r="909" customHeight="1" spans="1:1">
-      <c r="A909" s="58"/>
+      <c r="A909" s="59"/>
     </row>
     <row r="910" customHeight="1" spans="1:1">
-      <c r="A910" s="58"/>
+      <c r="A910" s="59"/>
     </row>
     <row r="911" customHeight="1" spans="1:1">
-      <c r="A911" s="58"/>
+      <c r="A911" s="59"/>
     </row>
     <row r="912" customHeight="1" spans="1:1">
-      <c r="A912" s="58"/>
+      <c r="A912" s="59"/>
     </row>
     <row r="913" customHeight="1" spans="1:1">
-      <c r="A913" s="58"/>
+      <c r="A913" s="59"/>
     </row>
     <row r="914" customHeight="1" spans="1:1">
-      <c r="A914" s="58"/>
+      <c r="A914" s="59"/>
     </row>
     <row r="915" customHeight="1" spans="1:1">
-      <c r="A915" s="58"/>
+      <c r="A915" s="59"/>
     </row>
     <row r="916" customHeight="1" spans="1:1">
-      <c r="A916" s="58"/>
+      <c r="A916" s="59"/>
     </row>
     <row r="917" customHeight="1" spans="1:1">
-      <c r="A917" s="58"/>
+      <c r="A917" s="59"/>
     </row>
     <row r="918" customHeight="1" spans="1:1">
-      <c r="A918" s="58"/>
+      <c r="A918" s="59"/>
     </row>
     <row r="919" customHeight="1" spans="1:1">
-      <c r="A919" s="58"/>
+      <c r="A919" s="59"/>
     </row>
     <row r="920" customHeight="1" spans="1:1">
-      <c r="A920" s="58"/>
+      <c r="A920" s="59"/>
     </row>
     <row r="921" customHeight="1" spans="1:1">
-      <c r="A921" s="58"/>
+      <c r="A921" s="59"/>
     </row>
     <row r="922" customHeight="1" spans="1:1">
-      <c r="A922" s="58"/>
+      <c r="A922" s="59"/>
     </row>
     <row r="923" customHeight="1" spans="1:1">
-      <c r="A923" s="58"/>
+      <c r="A923" s="59"/>
     </row>
     <row r="924" customHeight="1" spans="1:1">
-      <c r="A924" s="58"/>
+      <c r="A924" s="59"/>
     </row>
     <row r="925" customHeight="1" spans="1:1">
-      <c r="A925" s="58"/>
+      <c r="A925" s="59"/>
     </row>
     <row r="926" customHeight="1" spans="1:1">
-      <c r="A926" s="58"/>
+      <c r="A926" s="59"/>
     </row>
     <row r="927" customHeight="1" spans="1:1">
-      <c r="A927" s="58"/>
+      <c r="A927" s="59"/>
     </row>
     <row r="928" customHeight="1" spans="1:1">
-      <c r="A928" s="58"/>
+      <c r="A928" s="59"/>
     </row>
     <row r="929" customHeight="1" spans="1:1">
-      <c r="A929" s="58"/>
+      <c r="A929" s="59"/>
     </row>
     <row r="930" customHeight="1" spans="1:1">
-      <c r="A930" s="58"/>
+      <c r="A930" s="59"/>
     </row>
     <row r="931" customHeight="1" spans="1:1">
-      <c r="A931" s="58"/>
+      <c r="A931" s="59"/>
     </row>
     <row r="932" customHeight="1" spans="1:1">
-      <c r="A932" s="58"/>
+      <c r="A932" s="59"/>
     </row>
     <row r="933" customHeight="1" spans="1:1">
-      <c r="A933" s="58"/>
+      <c r="A933" s="59"/>
     </row>
     <row r="934" customHeight="1" spans="1:1">
-      <c r="A934" s="58"/>
+      <c r="A934" s="59"/>
     </row>
     <row r="935" customHeight="1" spans="1:1">
-      <c r="A935" s="58"/>
+      <c r="A935" s="59"/>
     </row>
     <row r="936" customHeight="1" spans="1:1">
-      <c r="A936" s="58"/>
+      <c r="A936" s="59"/>
     </row>
     <row r="937" customHeight="1" spans="1:1">
-      <c r="A937" s="58"/>
+      <c r="A937" s="59"/>
     </row>
     <row r="938" customHeight="1" spans="1:1">
-      <c r="A938" s="58"/>
+      <c r="A938" s="59"/>
     </row>
     <row r="939" customHeight="1" spans="1:1">
-      <c r="A939" s="58"/>
+      <c r="A939" s="59"/>
     </row>
     <row r="940" customHeight="1" spans="1:1">
-      <c r="A940" s="58"/>
+      <c r="A940" s="59"/>
     </row>
     <row r="941" customHeight="1" spans="1:1">
-      <c r="A941" s="58"/>
+      <c r="A941" s="59"/>
     </row>
     <row r="942" customHeight="1" spans="1:1">
-      <c r="A942" s="58"/>
+      <c r="A942" s="59"/>
     </row>
     <row r="943" customHeight="1" spans="1:1">
-      <c r="A943" s="58"/>
+      <c r="A943" s="59"/>
     </row>
     <row r="944" customHeight="1" spans="1:1">
-      <c r="A944" s="58"/>
+      <c r="A944" s="59"/>
     </row>
     <row r="945" customHeight="1" spans="1:1">
-      <c r="A945" s="58"/>
+      <c r="A945" s="59"/>
     </row>
     <row r="946" customHeight="1" spans="1:1">
-      <c r="A946" s="58"/>
+      <c r="A946" s="59"/>
     </row>
     <row r="947" customHeight="1" spans="1:1">
-      <c r="A947" s="58"/>
+      <c r="A947" s="59"/>
     </row>
     <row r="948" customHeight="1" spans="1:1">
-      <c r="A948" s="58"/>
+      <c r="A948" s="59"/>
     </row>
     <row r="949" customHeight="1" spans="1:1">
-      <c r="A949" s="58"/>
+      <c r="A949" s="59"/>
     </row>
     <row r="950" customHeight="1" spans="1:1">
-      <c r="A950" s="58"/>
+      <c r="A950" s="59"/>
     </row>
     <row r="951" customHeight="1" spans="1:1">
-      <c r="A951" s="58"/>
+      <c r="A951" s="59"/>
     </row>
     <row r="952" customHeight="1" spans="1:1">
-      <c r="A952" s="58"/>
+      <c r="A952" s="59"/>
     </row>
     <row r="953" customHeight="1" spans="1:1">
-      <c r="A953" s="58"/>
+      <c r="A953" s="59"/>
     </row>
     <row r="954" customHeight="1" spans="1:1">
-      <c r="A954" s="58"/>
+      <c r="A954" s="59"/>
     </row>
     <row r="955" customHeight="1" spans="1:1">
-      <c r="A955" s="58"/>
+      <c r="A955" s="59"/>
     </row>
     <row r="956" customHeight="1" spans="1:1">
-      <c r="A956" s="58"/>
+      <c r="A956" s="59"/>
     </row>
     <row r="957" customHeight="1" spans="1:1">
-      <c r="A957" s="58"/>
+      <c r="A957" s="59"/>
     </row>
     <row r="958" customHeight="1" spans="1:1">
-      <c r="A958" s="58"/>
+      <c r="A958" s="59"/>
     </row>
     <row r="959" customHeight="1" spans="1:1">
-      <c r="A959" s="58"/>
+      <c r="A959" s="59"/>
     </row>
     <row r="960" customHeight="1" spans="1:1">
-      <c r="A960" s="58"/>
+      <c r="A960" s="59"/>
     </row>
     <row r="961" customHeight="1" spans="1:1">
-      <c r="A961" s="58"/>
+      <c r="A961" s="59"/>
     </row>
     <row r="962" customHeight="1" spans="1:1">
-      <c r="A962" s="58"/>
+      <c r="A962" s="59"/>
     </row>
     <row r="963" customHeight="1" spans="1:1">
-      <c r="A963" s="58"/>
+      <c r="A963" s="59"/>
     </row>
     <row r="964" customHeight="1" spans="1:1">
-      <c r="A964" s="58"/>
+      <c r="A964" s="59"/>
     </row>
     <row r="965" customHeight="1" spans="1:1">
-      <c r="A965" s="58"/>
+      <c r="A965" s="59"/>
     </row>
     <row r="966" customHeight="1" spans="1:1">
-      <c r="A966" s="58"/>
+      <c r="A966" s="59"/>
     </row>
     <row r="967" customHeight="1" spans="1:1">
-      <c r="A967" s="58"/>
+      <c r="A967" s="59"/>
     </row>
     <row r="968" customHeight="1" spans="1:1">
-      <c r="A968" s="58"/>
+      <c r="A968" s="59"/>
     </row>
     <row r="969" customHeight="1" spans="1:1">
-      <c r="A969" s="58"/>
+      <c r="A969" s="59"/>
     </row>
     <row r="970" customHeight="1" spans="1:1">
-      <c r="A970" s="58"/>
+      <c r="A970" s="59"/>
     </row>
     <row r="971" customHeight="1" spans="1:1">
-      <c r="A971" s="58"/>
+      <c r="A971" s="59"/>
     </row>
     <row r="972" customHeight="1" spans="1:1">
-      <c r="A972" s="58"/>
+      <c r="A972" s="59"/>
     </row>
     <row r="973" customHeight="1" spans="1:1">
-      <c r="A973" s="58"/>
+      <c r="A973" s="59"/>
     </row>
     <row r="974" customHeight="1" spans="1:1">
-      <c r="A974" s="58"/>
+      <c r="A974" s="59"/>
     </row>
     <row r="975" customHeight="1" spans="1:1">
-      <c r="A975" s="58"/>
+      <c r="A975" s="59"/>
     </row>
     <row r="976" customHeight="1" spans="1:1">
-      <c r="A976" s="58"/>
+      <c r="A976" s="59"/>
     </row>
     <row r="977" customHeight="1" spans="1:1">
-      <c r="A977" s="58"/>
+      <c r="A977" s="59"/>
     </row>
     <row r="978" customHeight="1" spans="1:1">
-      <c r="A978" s="58"/>
+      <c r="A978" s="59"/>
     </row>
     <row r="979" customHeight="1" spans="1:1">
-      <c r="A979" s="58"/>
+      <c r="A979" s="59"/>
     </row>
     <row r="980" customHeight="1" spans="1:1">
-      <c r="A980" s="58"/>
+      <c r="A980" s="59"/>
     </row>
     <row r="981" customHeight="1" spans="1:1">
-      <c r="A981" s="58"/>
+      <c r="A981" s="59"/>
     </row>
     <row r="982" customHeight="1" spans="1:1">
-      <c r="A982" s="58"/>
+      <c r="A982" s="59"/>
     </row>
     <row r="983" customHeight="1" spans="1:1">
-      <c r="A983" s="58"/>
+      <c r="A983" s="59"/>
     </row>
     <row r="984" customHeight="1" spans="1:1">
-      <c r="A984" s="58"/>
+      <c r="A984" s="59"/>
     </row>
     <row r="985" customHeight="1" spans="1:1">
-      <c r="A985" s="58"/>
+      <c r="A985" s="59"/>
     </row>
     <row r="986" customHeight="1" spans="1:1">
-      <c r="A986" s="58"/>
+      <c r="A986" s="59"/>
     </row>
     <row r="987" customHeight="1" spans="1:1">
-      <c r="A987" s="58"/>
+      <c r="A987" s="59"/>
     </row>
     <row r="988" customHeight="1" spans="1:1">
-      <c r="A988" s="58"/>
+      <c r="A988" s="59"/>
     </row>
     <row r="989" customHeight="1" spans="1:1">
-      <c r="A989" s="58"/>
+      <c r="A989" s="59"/>
     </row>
     <row r="990" customHeight="1" spans="1:1">
-      <c r="A990" s="58"/>
+      <c r="A990" s="59"/>
     </row>
     <row r="991" customHeight="1" spans="1:1">
-      <c r="A991" s="58"/>
+      <c r="A991" s="59"/>
     </row>
     <row r="992" customHeight="1" spans="1:1">
-      <c r="A992" s="58"/>
+      <c r="A992" s="59"/>
     </row>
     <row r="993" customHeight="1" spans="1:1">
-      <c r="A993" s="58"/>
+      <c r="A993" s="59"/>
     </row>
     <row r="994" customHeight="1" spans="1:1">
-      <c r="A994" s="58"/>
+      <c r="A994" s="59"/>
     </row>
     <row r="995" customHeight="1" spans="1:1">
-      <c r="A995" s="58"/>
+      <c r="A995" s="59"/>
     </row>
     <row r="996" customHeight="1" spans="1:1">
-      <c r="A996" s="58"/>
+      <c r="A996" s="59"/>
     </row>
     <row r="997" customHeight="1" spans="1:1">
-      <c r="A997" s="58"/>
+      <c r="A997" s="59"/>
     </row>
     <row r="998" customHeight="1" spans="1:1">
-      <c r="A998" s="58"/>
+      <c r="A998" s="59"/>
     </row>
     <row r="999" customHeight="1" spans="1:1">
-      <c r="A999" s="58"/>
+      <c r="A999" s="59"/>
     </row>
     <row r="1000" customHeight="1" spans="1:1">
-      <c r="A1000" s="58"/>
+      <c r="A1000" s="59"/>
     </row>
     <row r="1001" customHeight="1" spans="1:1">
-      <c r="A1001" s="58"/>
+      <c r="A1001" s="59"/>
     </row>
     <row r="1002" customHeight="1" spans="1:1">
-      <c r="A1002" s="58"/>
+      <c r="A1002" s="59"/>
     </row>
     <row r="1003" customHeight="1" spans="1:1">
-      <c r="A1003" s="58"/>
+      <c r="A1003" s="59"/>
     </row>
     <row r="1004" customHeight="1" spans="1:1">
-      <c r="A1004" s="58"/>
+      <c r="A1004" s="59"/>
     </row>
     <row r="1005" customHeight="1" spans="1:1">
-      <c r="A1005" s="58"/>
+      <c r="A1005" s="59"/>
     </row>
     <row r="1006" customHeight="1" spans="1:1">
-      <c r="A1006" s="58"/>
+      <c r="A1006" s="59"/>
     </row>
     <row r="1007" customHeight="1" spans="1:1">
-      <c r="A1007" s="58"/>
+      <c r="A1007" s="59"/>
     </row>
     <row r="1008" customHeight="1" spans="1:1">
-      <c r="A1008" s="58"/>
+      <c r="A1008" s="59"/>
     </row>
     <row r="1009" customHeight="1" spans="1:1">
-      <c r="A1009" s="58"/>
+      <c r="A1009" s="59"/>
     </row>
     <row r="1010" customHeight="1" spans="1:1">
-      <c r="A1010" s="58"/>
+      <c r="A1010" s="59"/>
     </row>
     <row r="1011" customHeight="1" spans="1:1">
-      <c r="A1011" s="58"/>
+      <c r="A1011" s="59"/>
     </row>
     <row r="1012" customHeight="1" spans="1:1">
-      <c r="A1012" s="58"/>
+      <c r="A1012" s="59"/>
     </row>
     <row r="1013" customHeight="1" spans="1:1">
-      <c r="A1013" s="58"/>
+      <c r="A1013" s="59"/>
     </row>
     <row r="1014" customHeight="1" spans="1:1">
-      <c r="A1014" s="58"/>
+      <c r="A1014" s="59"/>
     </row>
     <row r="1015" customHeight="1" spans="1:1">
-      <c r="A1015" s="58"/>
+      <c r="A1015" s="59"/>
     </row>
     <row r="1016" customHeight="1" spans="1:1">
-      <c r="A1016" s="58"/>
+      <c r="A1016" s="59"/>
     </row>
     <row r="1017" customHeight="1" spans="1:1">
-      <c r="A1017" s="58"/>
+      <c r="A1017" s="59"/>
     </row>
     <row r="1018" customHeight="1" spans="1:1">
-      <c r="A1018" s="58"/>
+      <c r="A1018" s="59"/>
     </row>
     <row r="1019" customHeight="1" spans="1:1">
-      <c r="A1019" s="58"/>
+      <c r="A1019" s="59"/>
     </row>
     <row r="1020" customHeight="1" spans="1:1">
-      <c r="A1020" s="58"/>
+      <c r="A1020" s="59"/>
     </row>
     <row r="1021" customHeight="1" spans="1:1">
-      <c r="A1021" s="58"/>
+      <c r="A1021" s="59"/>
     </row>
     <row r="1022" customHeight="1" spans="1:1">
-      <c r="A1022" s="58"/>
+      <c r="A1022" s="59"/>
     </row>
     <row r="1023" customHeight="1" spans="1:1">
-      <c r="A1023" s="58"/>
+      <c r="A1023" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>